<commit_message>
added spike data and eda
</commit_message>
<xml_diff>
--- a/analysis/lfp_rawdata_affiliative.xlsx
+++ b/analysis/lfp_rawdata_affiliative.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project- Electro\social_behavior_electro\analysis\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{586D3FEA-F65E-40BB-B0D8-62F02F034C11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -178,12 +184,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -191,7 +197,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -231,8 +237,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -242,13 +251,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -286,7 +303,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -320,6 +337,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -354,9 +372,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -529,232 +548,237 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CC38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="87" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:81">
+    <row r="1" spans="1:81" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1" t="s">
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1" t="s">
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-      <c r="AA1" s="1"/>
-      <c r="AB1" s="1"/>
-      <c r="AC1" s="1"/>
-      <c r="AD1" s="1"/>
-      <c r="AE1" s="1"/>
-      <c r="AF1" s="1" t="s">
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+      <c r="AA1" s="2"/>
+      <c r="AB1" s="2"/>
+      <c r="AC1" s="2"/>
+      <c r="AD1" s="2"/>
+      <c r="AE1" s="2"/>
+      <c r="AF1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="AG1" s="1"/>
-      <c r="AH1" s="1"/>
-      <c r="AI1" s="1"/>
-      <c r="AJ1" s="1"/>
-      <c r="AK1" s="1"/>
-      <c r="AL1" s="1"/>
-      <c r="AM1" s="1"/>
-      <c r="AN1" s="1"/>
-      <c r="AO1" s="1"/>
-      <c r="AP1" s="1" t="s">
+      <c r="AG1" s="2"/>
+      <c r="AH1" s="2"/>
+      <c r="AI1" s="2"/>
+      <c r="AJ1" s="2"/>
+      <c r="AK1" s="2"/>
+      <c r="AL1" s="2"/>
+      <c r="AM1" s="2"/>
+      <c r="AN1" s="2"/>
+      <c r="AO1" s="2"/>
+      <c r="AP1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="AQ1" s="1"/>
-      <c r="AR1" s="1"/>
-      <c r="AS1" s="1"/>
-      <c r="AT1" s="1"/>
-      <c r="AU1" s="1"/>
-      <c r="AV1" s="1"/>
-      <c r="AW1" s="1"/>
-      <c r="AX1" s="1"/>
-      <c r="AY1" s="1"/>
-      <c r="AZ1" s="1" t="s">
+      <c r="AQ1" s="2"/>
+      <c r="AR1" s="2"/>
+      <c r="AS1" s="2"/>
+      <c r="AT1" s="2"/>
+      <c r="AU1" s="2"/>
+      <c r="AV1" s="2"/>
+      <c r="AW1" s="2"/>
+      <c r="AX1" s="2"/>
+      <c r="AY1" s="2"/>
+      <c r="AZ1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="BA1" s="1"/>
-      <c r="BB1" s="1"/>
-      <c r="BC1" s="1"/>
-      <c r="BD1" s="1"/>
-      <c r="BE1" s="1"/>
-      <c r="BF1" s="1"/>
-      <c r="BG1" s="1"/>
-      <c r="BH1" s="1"/>
-      <c r="BI1" s="1"/>
-      <c r="BJ1" s="1" t="s">
+      <c r="BA1" s="2"/>
+      <c r="BB1" s="2"/>
+      <c r="BC1" s="2"/>
+      <c r="BD1" s="2"/>
+      <c r="BE1" s="2"/>
+      <c r="BF1" s="2"/>
+      <c r="BG1" s="2"/>
+      <c r="BH1" s="2"/>
+      <c r="BI1" s="2"/>
+      <c r="BJ1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="BK1" s="1"/>
-      <c r="BL1" s="1"/>
-      <c r="BM1" s="1"/>
-      <c r="BN1" s="1"/>
-      <c r="BO1" s="1"/>
-      <c r="BP1" s="1"/>
-      <c r="BQ1" s="1"/>
-      <c r="BR1" s="1"/>
-      <c r="BS1" s="1"/>
-      <c r="BT1" s="1" t="s">
+      <c r="BK1" s="2"/>
+      <c r="BL1" s="2"/>
+      <c r="BM1" s="2"/>
+      <c r="BN1" s="2"/>
+      <c r="BO1" s="2"/>
+      <c r="BP1" s="2"/>
+      <c r="BQ1" s="2"/>
+      <c r="BR1" s="2"/>
+      <c r="BS1" s="2"/>
+      <c r="BT1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="BU1" s="1"/>
-      <c r="BV1" s="1"/>
-      <c r="BW1" s="1"/>
-      <c r="BX1" s="1"/>
-      <c r="BY1" s="1"/>
-      <c r="BZ1" s="1"/>
-      <c r="CA1" s="1"/>
-      <c r="CB1" s="1"/>
-      <c r="CC1" s="1"/>
+      <c r="BU1" s="2"/>
+      <c r="BV1" s="2"/>
+      <c r="BW1" s="2"/>
+      <c r="BX1" s="2"/>
+      <c r="BY1" s="2"/>
+      <c r="BZ1" s="2"/>
+      <c r="CA1" s="2"/>
+      <c r="CB1" s="2"/>
+      <c r="CC1" s="2"/>
     </row>
-    <row r="2" spans="1:81">
+    <row r="2" spans="1:81" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1" t="s">
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1" t="s">
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1" t="s">
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-      <c r="AA2" s="1" t="s">
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="AB2" s="1"/>
-      <c r="AC2" s="1"/>
-      <c r="AD2" s="1"/>
-      <c r="AE2" s="1"/>
-      <c r="AF2" s="1" t="s">
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="2"/>
+      <c r="AF2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="AG2" s="1"/>
-      <c r="AH2" s="1"/>
-      <c r="AI2" s="1"/>
-      <c r="AJ2" s="1"/>
-      <c r="AK2" s="1" t="s">
+      <c r="AG2" s="2"/>
+      <c r="AH2" s="2"/>
+      <c r="AI2" s="2"/>
+      <c r="AJ2" s="2"/>
+      <c r="AK2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="AL2" s="1"/>
-      <c r="AM2" s="1"/>
-      <c r="AN2" s="1"/>
-      <c r="AO2" s="1"/>
-      <c r="AP2" s="1" t="s">
+      <c r="AL2" s="2"/>
+      <c r="AM2" s="2"/>
+      <c r="AN2" s="2"/>
+      <c r="AO2" s="2"/>
+      <c r="AP2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="AQ2" s="1"/>
-      <c r="AR2" s="1"/>
-      <c r="AS2" s="1"/>
-      <c r="AT2" s="1"/>
-      <c r="AU2" s="1" t="s">
+      <c r="AQ2" s="2"/>
+      <c r="AR2" s="2"/>
+      <c r="AS2" s="2"/>
+      <c r="AT2" s="2"/>
+      <c r="AU2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="AV2" s="1"/>
-      <c r="AW2" s="1"/>
-      <c r="AX2" s="1"/>
-      <c r="AY2" s="1"/>
-      <c r="AZ2" s="1" t="s">
+      <c r="AV2" s="2"/>
+      <c r="AW2" s="2"/>
+      <c r="AX2" s="2"/>
+      <c r="AY2" s="2"/>
+      <c r="AZ2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="BA2" s="1"/>
-      <c r="BB2" s="1"/>
-      <c r="BC2" s="1"/>
-      <c r="BD2" s="1"/>
-      <c r="BE2" s="1" t="s">
+      <c r="BA2" s="2"/>
+      <c r="BB2" s="2"/>
+      <c r="BC2" s="2"/>
+      <c r="BD2" s="2"/>
+      <c r="BE2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="BF2" s="1"/>
-      <c r="BG2" s="1"/>
-      <c r="BH2" s="1"/>
-      <c r="BI2" s="1"/>
-      <c r="BJ2" s="1" t="s">
+      <c r="BF2" s="2"/>
+      <c r="BG2" s="2"/>
+      <c r="BH2" s="2"/>
+      <c r="BI2" s="2"/>
+      <c r="BJ2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="BK2" s="1"/>
-      <c r="BL2" s="1"/>
-      <c r="BM2" s="1"/>
-      <c r="BN2" s="1"/>
-      <c r="BO2" s="1" t="s">
+      <c r="BK2" s="2"/>
+      <c r="BL2" s="2"/>
+      <c r="BM2" s="2"/>
+      <c r="BN2" s="2"/>
+      <c r="BO2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="BP2" s="1"/>
-      <c r="BQ2" s="1"/>
-      <c r="BR2" s="1"/>
-      <c r="BS2" s="1"/>
-      <c r="BT2" s="1" t="s">
+      <c r="BP2" s="2"/>
+      <c r="BQ2" s="2"/>
+      <c r="BR2" s="2"/>
+      <c r="BS2" s="2"/>
+      <c r="BT2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="BU2" s="1"/>
-      <c r="BV2" s="1"/>
-      <c r="BW2" s="1"/>
-      <c r="BX2" s="1"/>
-      <c r="BY2" s="1" t="s">
+      <c r="BU2" s="2"/>
+      <c r="BV2" s="2"/>
+      <c r="BW2" s="2"/>
+      <c r="BX2" s="2"/>
+      <c r="BY2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="BZ2" s="1"/>
-      <c r="CA2" s="1"/>
-      <c r="CB2" s="1"/>
-      <c r="CC2" s="1"/>
+      <c r="BZ2" s="2"/>
+      <c r="CA2" s="2"/>
+      <c r="CB2" s="2"/>
+      <c r="CC2" s="2"/>
     </row>
-    <row r="3" spans="1:81">
+    <row r="3" spans="1:81" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -999,12 +1023,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:81">
+    <row r="4" spans="1:81" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:81">
+    <row r="5" spans="1:81" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
@@ -1012,70 +1036,70 @@
         <v>5.165</v>
       </c>
       <c r="M5">
-        <v>6.9304</v>
+        <v>6.9303999999999997</v>
       </c>
       <c r="N5">
-        <v>5.7226</v>
+        <v>5.7225999999999999</v>
       </c>
       <c r="O5">
-        <v>1.7654</v>
+        <v>1.7654000000000001</v>
       </c>
       <c r="P5">
-        <v>0.5575999999999999</v>
+        <v>0.55759999999999987</v>
       </c>
       <c r="Q5">
-        <v>21.0125</v>
+        <v>21.012499999999999</v>
       </c>
       <c r="R5">
-        <v>24.5189</v>
+        <v>24.518899999999999</v>
       </c>
       <c r="S5">
         <v>22.3993</v>
       </c>
       <c r="T5">
-        <v>3.506399999999999</v>
+        <v>3.5063999999999989</v>
       </c>
       <c r="U5">
-        <v>1.386800000000001</v>
+        <v>1.3868000000000009</v>
       </c>
       <c r="AP5">
-        <v>8.3833</v>
+        <v>8.3833000000000002</v>
       </c>
       <c r="AQ5">
-        <v>9.5184</v>
+        <v>9.5183999999999997</v>
       </c>
       <c r="AR5">
-        <v>8.713100000000001</v>
+        <v>8.7131000000000007</v>
       </c>
       <c r="AS5">
         <v>1.1351</v>
       </c>
       <c r="AT5">
-        <v>0.3298000000000005</v>
+        <v>0.32980000000000048</v>
       </c>
       <c r="AU5">
-        <v>20.8778</v>
+        <v>20.877800000000001</v>
       </c>
       <c r="AV5">
         <v>24.3931</v>
       </c>
       <c r="AW5">
-        <v>22.295</v>
+        <v>22.295000000000002</v>
       </c>
       <c r="AX5">
-        <v>3.5153</v>
+        <v>3.5152999999999999</v>
       </c>
       <c r="AY5">
-        <v>1.417200000000001</v>
+        <v>1.4172000000000009</v>
       </c>
       <c r="AZ5">
-        <v>8.7372</v>
+        <v>8.7371999999999996</v>
       </c>
       <c r="BA5">
-        <v>10.1232</v>
+        <v>10.123200000000001</v>
       </c>
       <c r="BB5">
-        <v>9.295299999999999</v>
+        <v>9.2952999999999992</v>
       </c>
       <c r="BC5">
         <v>1.386000000000001</v>
@@ -1087,27 +1111,27 @@
         <v>20.302</v>
       </c>
       <c r="BF5">
-        <v>24.0113</v>
+        <v>24.011299999999999</v>
       </c>
       <c r="BG5">
         <v>21.7654</v>
       </c>
       <c r="BH5">
-        <v>3.709299999999999</v>
+        <v>3.7092999999999989</v>
       </c>
       <c r="BI5">
         <v>1.4634</v>
       </c>
     </row>
-    <row r="6" spans="1:81">
+    <row r="6" spans="1:81" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B6">
-        <v>3.6141</v>
+        <v>3.6141000000000001</v>
       </c>
       <c r="C6">
-        <v>4.743</v>
+        <v>4.7430000000000003</v>
       </c>
       <c r="D6">
         <v>3.68</v>
@@ -1116,85 +1140,85 @@
         <v>1.1289</v>
       </c>
       <c r="F6">
-        <v>0.06590000000000007</v>
+        <v>6.590000000000007E-2</v>
       </c>
       <c r="G6">
         <v>19.2028</v>
       </c>
       <c r="H6">
-        <v>24.6101</v>
+        <v>24.610099999999999</v>
       </c>
       <c r="I6">
-        <v>20.1593</v>
+        <v>20.159300000000002</v>
       </c>
       <c r="J6">
-        <v>5.407299999999999</v>
+        <v>5.4072999999999993</v>
       </c>
       <c r="K6">
         <v>0.9565000000000019</v>
       </c>
       <c r="AP6">
-        <v>4.0858</v>
+        <v>4.0857999999999999</v>
       </c>
       <c r="AQ6">
-        <v>5.1362</v>
+        <v>5.1361999999999997</v>
       </c>
       <c r="AR6">
-        <v>4.1968</v>
+        <v>4.1967999999999996</v>
       </c>
       <c r="AS6">
         <v>1.0504</v>
       </c>
       <c r="AT6">
-        <v>0.1109999999999998</v>
+        <v>0.11099999999999979</v>
       </c>
       <c r="AU6">
         <v>19.2622</v>
       </c>
       <c r="AV6">
-        <v>24.6093</v>
+        <v>24.609300000000001</v>
       </c>
       <c r="AW6">
         <v>20.0487</v>
       </c>
       <c r="AX6">
-        <v>5.347100000000001</v>
+        <v>5.3471000000000011</v>
       </c>
       <c r="AY6">
         <v>0.7865000000000002</v>
       </c>
       <c r="BT6">
-        <v>4.279</v>
+        <v>4.2789999999999999</v>
       </c>
       <c r="BU6">
-        <v>5.3541</v>
+        <v>5.3540999999999999</v>
       </c>
       <c r="BV6">
-        <v>4.2937</v>
+        <v>4.2937000000000003</v>
       </c>
       <c r="BW6">
-        <v>1.0751</v>
+        <v>1.0750999999999999</v>
       </c>
       <c r="BX6">
-        <v>0.01470000000000038</v>
+        <v>1.4700000000000379E-2</v>
       </c>
       <c r="BY6">
-        <v>19.5918</v>
+        <v>19.591799999999999</v>
       </c>
       <c r="BZ6">
-        <v>24.8878</v>
+        <v>24.887799999999999</v>
       </c>
       <c r="CA6">
         <v>20.6784</v>
       </c>
       <c r="CB6">
-        <v>5.295999999999999</v>
+        <v>5.2959999999999994</v>
       </c>
       <c r="CC6">
-        <v>1.086600000000001</v>
+        <v>1.0866000000000009</v>
       </c>
     </row>
-    <row r="7" spans="1:81">
+    <row r="7" spans="1:81" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -1202,49 +1226,49 @@
         <v>1.9454</v>
       </c>
       <c r="C7">
-        <v>3.4285</v>
+        <v>3.4285000000000001</v>
       </c>
       <c r="D7">
         <v>2.3975</v>
       </c>
       <c r="E7">
-        <v>1.4831</v>
+        <v>1.4831000000000001</v>
       </c>
       <c r="F7">
-        <v>0.4520999999999999</v>
+        <v>0.45209999999999989</v>
       </c>
       <c r="G7">
         <v>16.2575</v>
       </c>
       <c r="H7">
-        <v>19.1835</v>
+        <v>19.183499999999999</v>
       </c>
       <c r="I7">
         <v>16.9894</v>
       </c>
       <c r="J7">
-        <v>2.925999999999998</v>
+        <v>2.9259999999999979</v>
       </c>
       <c r="K7">
-        <v>0.7318999999999996</v>
+        <v>0.73189999999999955</v>
       </c>
       <c r="AP7">
-        <v>2.333</v>
+        <v>2.3330000000000002</v>
       </c>
       <c r="AQ7">
-        <v>3.7311</v>
+        <v>3.7311000000000001</v>
       </c>
       <c r="AR7">
         <v>2.8</v>
       </c>
       <c r="AS7">
-        <v>1.3981</v>
+        <v>1.3980999999999999</v>
       </c>
       <c r="AT7">
-        <v>0.4669999999999996</v>
+        <v>0.46699999999999958</v>
       </c>
       <c r="AU7">
-        <v>16.4259</v>
+        <v>16.425899999999999</v>
       </c>
       <c r="AV7">
         <v>19.3537</v>
@@ -1253,43 +1277,43 @@
         <v>17.0565</v>
       </c>
       <c r="AX7">
-        <v>2.927800000000001</v>
+        <v>2.9278000000000008</v>
       </c>
       <c r="AY7">
-        <v>0.6306000000000012</v>
+        <v>0.63060000000000116</v>
       </c>
       <c r="BT7">
         <v>2.3024</v>
       </c>
       <c r="BU7">
-        <v>3.7144</v>
+        <v>3.7143999999999999</v>
       </c>
       <c r="BV7">
-        <v>2.6719</v>
+        <v>2.6718999999999999</v>
       </c>
       <c r="BW7">
-        <v>1.412</v>
+        <v>1.4119999999999999</v>
       </c>
       <c r="BX7">
-        <v>0.3694999999999999</v>
+        <v>0.36949999999999988</v>
       </c>
       <c r="BY7">
-        <v>16.6628</v>
+        <v>16.662800000000001</v>
       </c>
       <c r="BZ7">
-        <v>19.5052</v>
+        <v>19.505199999999999</v>
       </c>
       <c r="CA7">
-        <v>17.5729</v>
+        <v>17.572900000000001</v>
       </c>
       <c r="CB7">
-        <v>2.842399999999998</v>
+        <v>2.8423999999999978</v>
       </c>
       <c r="CC7">
-        <v>0.9100999999999999</v>
+        <v>0.91009999999999991</v>
       </c>
     </row>
-    <row r="8" spans="1:81">
+    <row r="8" spans="1:81" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
@@ -1300,58 +1324,58 @@
         <v>13.7319</v>
       </c>
       <c r="D8">
-        <v>13.9432</v>
+        <v>13.943199999999999</v>
       </c>
       <c r="E8">
-        <v>-0.1714000000000002</v>
+        <v>-0.17140000000000019</v>
       </c>
       <c r="F8">
-        <v>0.03989999999999938</v>
+        <v>3.989999999999938E-2</v>
       </c>
       <c r="G8">
-        <v>23.1668</v>
+        <v>23.166799999999999</v>
       </c>
       <c r="H8">
-        <v>22.5693</v>
+        <v>22.569299999999998</v>
       </c>
       <c r="I8">
-        <v>22.7137</v>
+        <v>22.713699999999999</v>
       </c>
       <c r="J8">
-        <v>-0.5975000000000001</v>
+        <v>-0.59750000000000014</v>
       </c>
       <c r="K8">
-        <v>-0.4530999999999992</v>
+        <v>-0.45309999999999923</v>
       </c>
       <c r="L8">
-        <v>5.6446</v>
+        <v>5.6445999999999996</v>
       </c>
       <c r="M8">
-        <v>5.6412</v>
+        <v>5.6412000000000004</v>
       </c>
       <c r="N8">
         <v>5.5987</v>
       </c>
       <c r="O8">
-        <v>-0.003399999999999181</v>
+        <v>-3.399999999999181E-3</v>
       </c>
       <c r="P8">
-        <v>-0.04589999999999961</v>
+        <v>-4.5899999999999608E-2</v>
       </c>
       <c r="Q8">
         <v>18.3461</v>
       </c>
       <c r="R8">
-        <v>17.8177</v>
+        <v>17.817699999999999</v>
       </c>
       <c r="S8">
-        <v>18.162</v>
+        <v>18.161999999999999</v>
       </c>
       <c r="T8">
-        <v>-0.5284000000000013</v>
+        <v>-0.52840000000000131</v>
       </c>
       <c r="U8">
-        <v>-0.1841000000000008</v>
+        <v>-0.18410000000000079</v>
       </c>
       <c r="V8">
         <v>6.6974</v>
@@ -1360,22 +1384,22 @@
         <v>6.7035</v>
       </c>
       <c r="X8">
-        <v>6.971</v>
+        <v>6.9710000000000001</v>
       </c>
       <c r="Y8">
-        <v>0.006099999999999994</v>
+        <v>6.0999999999999943E-3</v>
       </c>
       <c r="Z8">
-        <v>0.2736000000000001</v>
+        <v>0.27360000000000012</v>
       </c>
       <c r="AA8">
         <v>22.1006</v>
       </c>
       <c r="AB8">
-        <v>21.836</v>
+        <v>21.835999999999999</v>
       </c>
       <c r="AC8">
-        <v>22.3982</v>
+        <v>22.398199999999999</v>
       </c>
       <c r="AD8">
         <v>-0.2646000000000015</v>
@@ -1390,34 +1414,34 @@
         <v>14.8142</v>
       </c>
       <c r="BB8">
-        <v>14.9402</v>
+        <v>14.940200000000001</v>
       </c>
       <c r="BC8">
-        <v>-0.04490000000000016</v>
+        <v>-4.4900000000000162E-2</v>
       </c>
       <c r="BD8">
-        <v>0.08110000000000106</v>
+        <v>8.110000000000106E-2</v>
       </c>
       <c r="BE8">
-        <v>21.6696</v>
+        <v>21.669599999999999</v>
       </c>
       <c r="BF8">
-        <v>21.6228</v>
+        <v>21.622800000000002</v>
       </c>
       <c r="BG8">
-        <v>21.7893</v>
+        <v>21.789300000000001</v>
       </c>
       <c r="BH8">
-        <v>-0.04679999999999751</v>
+        <v>-4.679999999999751E-2</v>
       </c>
       <c r="BI8">
-        <v>0.1197000000000017</v>
+        <v>0.11970000000000169</v>
       </c>
       <c r="BT8">
-        <v>10.2251</v>
+        <v>10.225099999999999</v>
       </c>
       <c r="BU8">
-        <v>10.3455</v>
+        <v>10.345499999999999</v>
       </c>
       <c r="BV8">
         <v>10.3942</v>
@@ -1426,7 +1450,7 @@
         <v>0.1204000000000001</v>
       </c>
       <c r="BX8">
-        <v>0.1691000000000003</v>
+        <v>0.16910000000000031</v>
       </c>
       <c r="BY8">
         <v>22.0307</v>
@@ -1435,7 +1459,7 @@
         <v>21.7544</v>
       </c>
       <c r="CA8">
-        <v>22.1505</v>
+        <v>22.150500000000001</v>
       </c>
       <c r="CB8">
         <v>-0.2762999999999991</v>
@@ -1444,42 +1468,42 @@
         <v>0.1198000000000015</v>
       </c>
     </row>
-    <row r="9" spans="1:81">
+    <row r="9" spans="1:81" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
       <c r="L9">
-        <v>5.6897</v>
+        <v>5.6897000000000002</v>
       </c>
       <c r="M9">
-        <v>6.2779</v>
+        <v>6.2778999999999998</v>
       </c>
       <c r="N9">
-        <v>5.814</v>
+        <v>5.8140000000000001</v>
       </c>
       <c r="O9">
-        <v>0.5881999999999996</v>
+        <v>0.58819999999999961</v>
       </c>
       <c r="P9">
         <v>0.1242999999999999</v>
       </c>
       <c r="Q9">
-        <v>21.4449</v>
+        <v>21.444900000000001</v>
       </c>
       <c r="R9">
-        <v>22.7574</v>
+        <v>22.757400000000001</v>
       </c>
       <c r="S9">
-        <v>22.3427</v>
+        <v>22.342700000000001</v>
       </c>
       <c r="T9">
         <v>1.3125</v>
       </c>
       <c r="U9">
-        <v>0.8978000000000002</v>
+        <v>0.89780000000000015</v>
       </c>
       <c r="V9">
-        <v>4.1012</v>
+        <v>4.1012000000000004</v>
       </c>
       <c r="W9">
         <v>4.7401</v>
@@ -1488,102 +1512,102 @@
         <v>4.0762</v>
       </c>
       <c r="Y9">
-        <v>0.6388999999999996</v>
+        <v>0.63889999999999958</v>
       </c>
       <c r="Z9">
-        <v>-0.02500000000000036</v>
+        <v>-2.5000000000000359E-2</v>
       </c>
       <c r="AA9">
-        <v>19.8988</v>
+        <v>19.898800000000001</v>
       </c>
       <c r="AB9">
-        <v>19.6489</v>
+        <v>19.648900000000001</v>
       </c>
       <c r="AC9">
-        <v>20.0861</v>
+        <v>20.086099999999998</v>
       </c>
       <c r="AD9">
-        <v>-0.2499000000000002</v>
+        <v>-0.24990000000000021</v>
       </c>
       <c r="AE9">
-        <v>0.1872999999999969</v>
+        <v>0.18729999999999691</v>
       </c>
       <c r="BT9">
         <v>7.3182</v>
       </c>
       <c r="BU9">
-        <v>7.6965</v>
+        <v>7.6965000000000003</v>
       </c>
       <c r="BV9">
-        <v>7.2651</v>
+        <v>7.2651000000000003</v>
       </c>
       <c r="BW9">
         <v>0.3783000000000003</v>
       </c>
       <c r="BX9">
-        <v>-0.0530999999999997</v>
+        <v>-5.3099999999999703E-2</v>
       </c>
       <c r="BY9">
-        <v>23.065</v>
+        <v>23.065000000000001</v>
       </c>
       <c r="BZ9">
-        <v>23.8289</v>
+        <v>23.828900000000001</v>
       </c>
       <c r="CA9">
         <v>23.6068</v>
       </c>
       <c r="CB9">
-        <v>0.7638999999999996</v>
+        <v>0.76389999999999958</v>
       </c>
       <c r="CC9">
-        <v>0.5417999999999985</v>
+        <v>0.54179999999999851</v>
       </c>
     </row>
-    <row r="10" spans="1:81">
+    <row r="10" spans="1:81" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B10">
-        <v>9.772399999999999</v>
+        <v>9.7723999999999993</v>
       </c>
       <c r="C10">
-        <v>10.3846</v>
+        <v>10.384600000000001</v>
       </c>
       <c r="D10">
-        <v>9.465199999999999</v>
+        <v>9.4651999999999994</v>
       </c>
       <c r="E10">
-        <v>0.6122000000000014</v>
+        <v>0.61220000000000141</v>
       </c>
       <c r="F10">
-        <v>-0.3071999999999999</v>
+        <v>-0.30719999999999992</v>
       </c>
       <c r="G10">
         <v>20.4466</v>
       </c>
       <c r="H10">
-        <v>20.5893</v>
+        <v>20.589300000000001</v>
       </c>
       <c r="I10">
         <v>20.715</v>
       </c>
       <c r="J10">
-        <v>0.1427000000000014</v>
+        <v>0.14270000000000141</v>
       </c>
       <c r="K10">
-        <v>0.2683999999999997</v>
+        <v>0.26839999999999969</v>
       </c>
       <c r="L10">
-        <v>5.6614</v>
+        <v>5.6614000000000004</v>
       </c>
       <c r="M10">
-        <v>6.4214</v>
+        <v>6.4214000000000002</v>
       </c>
       <c r="N10">
-        <v>6.1755</v>
+        <v>6.1755000000000004</v>
       </c>
       <c r="O10">
-        <v>0.7599999999999998</v>
+        <v>0.75999999999999979</v>
       </c>
       <c r="P10">
         <v>0.5141</v>
@@ -1592,46 +1616,46 @@
         <v>22.1449</v>
       </c>
       <c r="R10">
-        <v>23.0843</v>
+        <v>23.084299999999999</v>
       </c>
       <c r="S10">
-        <v>22.2999</v>
+        <v>22.299900000000001</v>
       </c>
       <c r="T10">
-        <v>0.9393999999999991</v>
+        <v>0.93939999999999912</v>
       </c>
       <c r="U10">
-        <v>0.1550000000000011</v>
+        <v>0.15500000000000111</v>
       </c>
       <c r="V10">
-        <v>3.767</v>
+        <v>3.7669999999999999</v>
       </c>
       <c r="W10">
-        <v>4.3234</v>
+        <v>4.3234000000000004</v>
       </c>
       <c r="X10">
-        <v>4.0714</v>
+        <v>4.0713999999999997</v>
       </c>
       <c r="Y10">
-        <v>0.5564000000000004</v>
+        <v>0.55640000000000045</v>
       </c>
       <c r="Z10">
-        <v>0.3043999999999998</v>
+        <v>0.30439999999999978</v>
       </c>
       <c r="AA10">
-        <v>19.8851</v>
+        <v>19.885100000000001</v>
       </c>
       <c r="AB10">
-        <v>18.3683</v>
+        <v>18.368300000000001</v>
       </c>
       <c r="AC10">
-        <v>18.9493</v>
+        <v>18.949300000000001</v>
       </c>
       <c r="AD10">
-        <v>-1.5168</v>
+        <v>-1.5167999999999999</v>
       </c>
       <c r="AE10">
-        <v>-0.9358000000000004</v>
+        <v>-0.93580000000000041</v>
       </c>
       <c r="BT10">
         <v>11.1563</v>
@@ -1640,19 +1664,19 @@
         <v>11.3268</v>
       </c>
       <c r="BV10">
-        <v>10.5706</v>
+        <v>10.570600000000001</v>
       </c>
       <c r="BW10">
-        <v>0.1705000000000005</v>
+        <v>0.17050000000000051</v>
       </c>
       <c r="BX10">
-        <v>-0.5856999999999992</v>
+        <v>-0.58569999999999922</v>
       </c>
       <c r="BY10">
         <v>21.8582</v>
       </c>
       <c r="BZ10">
-        <v>22.5714</v>
+        <v>22.571400000000001</v>
       </c>
       <c r="CA10">
         <v>21.9224</v>
@@ -1661,42 +1685,42 @@
         <v>0.7132000000000005</v>
       </c>
       <c r="CC10">
-        <v>0.06419999999999959</v>
+        <v>6.4199999999999591E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:81">
+    <row r="11" spans="1:81" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
       <c r="V11">
-        <v>15.0545</v>
+        <v>15.054500000000001</v>
       </c>
       <c r="W11">
-        <v>14.7764</v>
+        <v>14.776400000000001</v>
       </c>
       <c r="X11">
         <v>14.8719</v>
       </c>
       <c r="Y11">
-        <v>-0.2781000000000002</v>
+        <v>-0.27810000000000018</v>
       </c>
       <c r="Z11">
-        <v>-0.1826000000000008</v>
+        <v>-0.18260000000000079</v>
       </c>
       <c r="AA11">
         <v>28.1631</v>
       </c>
       <c r="AB11">
-        <v>31.2887</v>
+        <v>31.288699999999999</v>
       </c>
       <c r="AC11">
-        <v>30.5881</v>
+        <v>30.588100000000001</v>
       </c>
       <c r="AD11">
         <v>3.125599999999999</v>
       </c>
       <c r="AE11">
-        <v>2.425000000000001</v>
+        <v>2.4250000000000012</v>
       </c>
       <c r="AF11">
         <v>12.1127</v>
@@ -1708,227 +1732,227 @@
         <v>12.1233</v>
       </c>
       <c r="AI11">
-        <v>0.7296999999999993</v>
+        <v>0.72969999999999935</v>
       </c>
       <c r="AJ11">
-        <v>0.01060000000000016</v>
+        <v>1.060000000000016E-2</v>
       </c>
       <c r="AK11">
-        <v>26.7527</v>
+        <v>26.752700000000001</v>
       </c>
       <c r="AL11">
-        <v>30.0599</v>
+        <v>30.059899999999999</v>
       </c>
       <c r="AM11">
-        <v>28.679</v>
+        <v>28.678999999999998</v>
       </c>
       <c r="AN11">
-        <v>3.307199999999998</v>
+        <v>3.3071999999999981</v>
       </c>
       <c r="AO11">
-        <v>1.926299999999998</v>
+        <v>1.9262999999999979</v>
       </c>
     </row>
-    <row r="12" spans="1:81">
+    <row r="12" spans="1:81" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
       <c r="L12">
-        <v>8.8546</v>
+        <v>8.8545999999999996</v>
       </c>
       <c r="M12">
-        <v>8.4663</v>
+        <v>8.4663000000000004</v>
       </c>
       <c r="N12">
-        <v>8.983499999999999</v>
+        <v>8.9834999999999994</v>
       </c>
       <c r="O12">
         <v>-0.3882999999999992</v>
       </c>
       <c r="P12">
-        <v>0.1288999999999998</v>
+        <v>0.12889999999999979</v>
       </c>
       <c r="Q12">
-        <v>21.4357</v>
+        <v>21.435700000000001</v>
       </c>
       <c r="R12">
-        <v>22.0332</v>
+        <v>22.033200000000001</v>
       </c>
       <c r="S12">
         <v>21.5046</v>
       </c>
       <c r="T12">
-        <v>0.5975000000000001</v>
+        <v>0.59750000000000014</v>
       </c>
       <c r="U12">
-        <v>0.0688999999999993</v>
+        <v>6.8899999999999295E-2</v>
       </c>
       <c r="V12">
-        <v>7.876</v>
+        <v>7.8760000000000003</v>
       </c>
       <c r="W12">
-        <v>7.7257</v>
+        <v>7.7256999999999998</v>
       </c>
       <c r="X12">
-        <v>8.0091</v>
+        <v>8.0091000000000001</v>
       </c>
       <c r="Y12">
-        <v>-0.1503000000000005</v>
+        <v>-0.15030000000000049</v>
       </c>
       <c r="Z12">
         <v>0.1330999999999998</v>
       </c>
       <c r="AA12">
-        <v>21.2497</v>
+        <v>21.249700000000001</v>
       </c>
       <c r="AB12">
-        <v>21.9926</v>
+        <v>21.992599999999999</v>
       </c>
       <c r="AC12">
-        <v>21.531</v>
+        <v>21.530999999999999</v>
       </c>
       <c r="AD12">
-        <v>0.7428999999999988</v>
+        <v>0.74289999999999878</v>
       </c>
       <c r="AE12">
-        <v>0.2812999999999981</v>
+        <v>0.28129999999999811</v>
       </c>
       <c r="AF12">
-        <v>5.3432</v>
+        <v>5.3432000000000004</v>
       </c>
       <c r="AG12">
-        <v>6.3017</v>
+        <v>6.3017000000000003</v>
       </c>
       <c r="AH12">
-        <v>5.0116</v>
+        <v>5.0115999999999996</v>
       </c>
       <c r="AI12">
-        <v>0.9584999999999999</v>
+        <v>0.95849999999999991</v>
       </c>
       <c r="AJ12">
-        <v>-0.3316000000000008</v>
+        <v>-0.33160000000000078</v>
       </c>
       <c r="AK12">
-        <v>21.8534</v>
+        <v>21.853400000000001</v>
       </c>
       <c r="AL12">
         <v>21.9312</v>
       </c>
       <c r="AM12">
-        <v>22.0526</v>
+        <v>22.052600000000002</v>
       </c>
       <c r="AN12">
-        <v>0.07779999999999987</v>
+        <v>7.7799999999999869E-2</v>
       </c>
       <c r="AO12">
-        <v>0.1992000000000012</v>
+        <v>0.19920000000000121</v>
       </c>
       <c r="AP12">
-        <v>7.7822</v>
+        <v>7.7821999999999996</v>
       </c>
       <c r="AQ12">
         <v>8.8971</v>
       </c>
       <c r="AR12">
-        <v>7.4027</v>
+        <v>7.4027000000000003</v>
       </c>
       <c r="AS12">
         <v>1.1149</v>
       </c>
       <c r="AT12">
-        <v>-0.3794999999999993</v>
+        <v>-0.37949999999999928</v>
       </c>
       <c r="AU12">
-        <v>21.5589</v>
+        <v>21.558900000000001</v>
       </c>
       <c r="AV12">
-        <v>20.764</v>
+        <v>20.763999999999999</v>
       </c>
       <c r="AW12">
-        <v>22.3531</v>
+        <v>22.353100000000001</v>
       </c>
       <c r="AX12">
-        <v>-0.7949000000000019</v>
+        <v>-0.79490000000000194</v>
       </c>
       <c r="AY12">
-        <v>0.7942</v>
+        <v>0.79420000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:81">
+    <row r="13" spans="1:81" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B13">
-        <v>7.8012</v>
+        <v>7.8011999999999997</v>
       </c>
       <c r="C13">
         <v>9.0122</v>
       </c>
       <c r="D13">
-        <v>8.6557</v>
+        <v>8.6556999999999995</v>
       </c>
       <c r="E13">
-        <v>1.211</v>
+        <v>1.2110000000000001</v>
       </c>
       <c r="F13">
-        <v>0.8544999999999998</v>
+        <v>0.85449999999999982</v>
       </c>
       <c r="G13">
         <v>21.1708</v>
       </c>
       <c r="H13">
-        <v>22.0645</v>
+        <v>22.064499999999999</v>
       </c>
       <c r="I13">
-        <v>22.2924</v>
+        <v>22.292400000000001</v>
       </c>
       <c r="J13">
-        <v>0.8936999999999991</v>
+        <v>0.89369999999999905</v>
       </c>
       <c r="K13">
         <v>1.121600000000001</v>
       </c>
       <c r="L13">
-        <v>5.453799999999999</v>
+        <v>5.4537999999999993</v>
       </c>
       <c r="M13">
-        <v>6.263199999999999</v>
+        <v>6.2631999999999994</v>
       </c>
       <c r="N13">
         <v>5.702</v>
       </c>
       <c r="O13">
-        <v>0.8094000000000001</v>
+        <v>0.80940000000000012</v>
       </c>
       <c r="P13">
-        <v>0.2482000000000006</v>
+        <v>0.24820000000000059</v>
       </c>
       <c r="Q13">
-        <v>20.1197</v>
+        <v>20.119700000000002</v>
       </c>
       <c r="R13">
-        <v>20.38415</v>
+        <v>20.384150000000002</v>
       </c>
       <c r="S13">
-        <v>20.6308</v>
+        <v>20.630800000000001</v>
       </c>
       <c r="T13">
-        <v>0.2644499999999965</v>
+        <v>0.26444999999999652</v>
       </c>
       <c r="U13">
         <v>0.511099999999999</v>
       </c>
       <c r="BT13">
-        <v>4.7849</v>
+        <v>4.7849000000000004</v>
       </c>
       <c r="BU13">
-        <v>7.1615</v>
+        <v>7.1615000000000002</v>
       </c>
       <c r="BV13">
-        <v>5.5233</v>
+        <v>5.5232999999999999</v>
       </c>
       <c r="BW13">
-        <v>2.3766</v>
+        <v>2.3765999999999998</v>
       </c>
       <c r="BX13">
         <v>0.7383999999999995</v>
@@ -1937,167 +1961,167 @@
         <v>19.7666</v>
       </c>
       <c r="BZ13">
-        <v>20.4034</v>
+        <v>20.403400000000001</v>
       </c>
       <c r="CA13">
-        <v>20.693</v>
+        <v>20.693000000000001</v>
       </c>
       <c r="CB13">
-        <v>0.6368000000000009</v>
+        <v>0.63680000000000092</v>
       </c>
       <c r="CC13">
         <v>0.926400000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:81">
+    <row r="14" spans="1:81" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B14">
-        <v>7.3089</v>
+        <v>7.3089000000000004</v>
       </c>
       <c r="C14">
-        <v>8.527900000000001</v>
+        <v>8.5279000000000007</v>
       </c>
       <c r="D14">
-        <v>7.5309</v>
+        <v>7.5308999999999999</v>
       </c>
       <c r="E14">
-        <v>1.219</v>
+        <v>1.2190000000000001</v>
       </c>
       <c r="F14">
         <v>0.2219999999999995</v>
       </c>
       <c r="G14">
-        <v>21.0557</v>
+        <v>21.055700000000002</v>
       </c>
       <c r="H14">
-        <v>21.0421</v>
+        <v>21.042100000000001</v>
       </c>
       <c r="I14">
         <v>21.4739</v>
       </c>
       <c r="J14">
-        <v>-0.01360000000000028</v>
+        <v>-1.360000000000028E-2</v>
       </c>
       <c r="K14">
-        <v>0.4181999999999988</v>
+        <v>0.41819999999999879</v>
       </c>
       <c r="L14">
-        <v>5.284</v>
+        <v>5.2839999999999998</v>
       </c>
       <c r="M14">
-        <v>5.5592</v>
+        <v>5.5591999999999997</v>
       </c>
       <c r="N14">
-        <v>4.1139</v>
+        <v>4.1139000000000001</v>
       </c>
       <c r="O14">
-        <v>0.2751999999999999</v>
+        <v>0.27519999999999989</v>
       </c>
       <c r="P14">
-        <v>-1.1701</v>
+        <v>-1.1700999999999999</v>
       </c>
       <c r="Q14">
-        <v>20.6161</v>
+        <v>20.616099999999999</v>
       </c>
       <c r="R14">
-        <v>20.9045</v>
+        <v>20.904499999999999</v>
       </c>
       <c r="S14">
-        <v>20.8207</v>
+        <v>20.820699999999999</v>
       </c>
       <c r="T14">
-        <v>0.2883999999999993</v>
+        <v>0.28839999999999932</v>
       </c>
       <c r="U14">
         <v>0.2045999999999992</v>
       </c>
       <c r="BT14">
-        <v>5.1381</v>
+        <v>5.1380999999999997</v>
       </c>
       <c r="BU14">
-        <v>6.4422</v>
+        <v>6.4421999999999997</v>
       </c>
       <c r="BV14">
-        <v>5.3217</v>
+        <v>5.3216999999999999</v>
       </c>
       <c r="BW14">
         <v>1.3041</v>
       </c>
       <c r="BX14">
-        <v>0.1836000000000002</v>
+        <v>0.18360000000000021</v>
       </c>
       <c r="BY14">
-        <v>18.0722</v>
+        <v>18.072199999999999</v>
       </c>
       <c r="BZ14">
-        <v>17.9868</v>
+        <v>17.986799999999999</v>
       </c>
       <c r="CA14">
         <v>18.977</v>
       </c>
       <c r="CB14">
-        <v>-0.08539999999999992</v>
+        <v>-8.539999999999992E-2</v>
       </c>
       <c r="CC14">
         <v>0.9048000000000016</v>
       </c>
     </row>
-    <row r="15" spans="1:81">
+    <row r="15" spans="1:81" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B15">
-        <v>4.5418</v>
+        <v>4.5418000000000003</v>
       </c>
       <c r="C15">
-        <v>5.3859</v>
+        <v>5.3859000000000004</v>
       </c>
       <c r="D15">
-        <v>5.0474</v>
+        <v>5.0473999999999997</v>
       </c>
       <c r="E15">
-        <v>0.8441000000000001</v>
+        <v>0.84410000000000007</v>
       </c>
       <c r="F15">
-        <v>0.5055999999999994</v>
+        <v>0.50559999999999938</v>
       </c>
       <c r="G15">
-        <v>18.7487</v>
+        <v>18.748699999999999</v>
       </c>
       <c r="H15">
-        <v>19.1369</v>
+        <v>19.136900000000001</v>
       </c>
       <c r="I15">
-        <v>19.7464</v>
+        <v>19.746400000000001</v>
       </c>
       <c r="J15">
-        <v>0.3882000000000012</v>
+        <v>0.38820000000000121</v>
       </c>
       <c r="K15">
-        <v>0.9977000000000018</v>
+        <v>0.99770000000000181</v>
       </c>
       <c r="L15">
-        <v>11.0431</v>
+        <v>11.043100000000001</v>
       </c>
       <c r="M15">
         <v>11.3431</v>
       </c>
       <c r="N15">
-        <v>10.9342</v>
+        <v>10.934200000000001</v>
       </c>
       <c r="O15">
-        <v>0.2999999999999989</v>
+        <v>0.29999999999999888</v>
       </c>
       <c r="P15">
         <v>-0.1089000000000002</v>
       </c>
       <c r="Q15">
-        <v>26.3617</v>
+        <v>26.361699999999999</v>
       </c>
       <c r="R15">
-        <v>26.4645</v>
+        <v>26.464500000000001</v>
       </c>
       <c r="S15">
         <v>27.03</v>
@@ -2106,49 +2130,49 @@
         <v>0.102800000000002</v>
       </c>
       <c r="U15">
-        <v>0.6683000000000021</v>
+        <v>0.66830000000000211</v>
       </c>
       <c r="V15">
-        <v>1.8683</v>
+        <v>1.8683000000000001</v>
       </c>
       <c r="W15">
-        <v>2.7809</v>
+        <v>2.7808999999999999</v>
       </c>
       <c r="X15">
-        <v>2.4094</v>
+        <v>2.4094000000000002</v>
       </c>
       <c r="Y15">
-        <v>0.9125999999999999</v>
+        <v>0.91259999999999986</v>
       </c>
       <c r="Z15">
-        <v>0.5411000000000001</v>
+        <v>0.54110000000000014</v>
       </c>
       <c r="AA15">
-        <v>17.094</v>
+        <v>17.094000000000001</v>
       </c>
       <c r="AB15">
-        <v>17.6196</v>
+        <v>17.619599999999998</v>
       </c>
       <c r="AC15">
-        <v>18.473</v>
+        <v>18.472999999999999</v>
       </c>
       <c r="AD15">
-        <v>0.5255999999999972</v>
+        <v>0.52559999999999718</v>
       </c>
       <c r="AE15">
         <v>1.378999999999998</v>
       </c>
       <c r="AF15">
-        <v>3.4748</v>
+        <v>3.4748000000000001</v>
       </c>
       <c r="AG15">
-        <v>4.386</v>
+        <v>4.3860000000000001</v>
       </c>
       <c r="AH15">
-        <v>4.0041</v>
+        <v>4.0041000000000002</v>
       </c>
       <c r="AI15">
-        <v>0.9112</v>
+        <v>0.91120000000000001</v>
       </c>
       <c r="AJ15">
         <v>0.5293000000000001</v>
@@ -2163,54 +2187,54 @@
         <v>19.1082</v>
       </c>
       <c r="AN15">
-        <v>0.3413000000000004</v>
+        <v>0.34130000000000038</v>
       </c>
       <c r="AO15">
         <v>1.2057</v>
       </c>
       <c r="BJ15">
-        <v>5.7767</v>
+        <v>5.7766999999999999</v>
       </c>
       <c r="BK15">
-        <v>6.728</v>
+        <v>6.7279999999999998</v>
       </c>
       <c r="BL15">
-        <v>6.3117</v>
+        <v>6.3117000000000001</v>
       </c>
       <c r="BM15">
-        <v>0.9512999999999998</v>
+        <v>0.95129999999999981</v>
       </c>
       <c r="BN15">
-        <v>0.5350000000000001</v>
+        <v>0.53500000000000014</v>
       </c>
       <c r="BO15">
         <v>22.7056</v>
       </c>
       <c r="BP15">
-        <v>23.3208</v>
+        <v>23.320799999999998</v>
       </c>
       <c r="BQ15">
-        <v>23.8011</v>
+        <v>23.801100000000002</v>
       </c>
       <c r="BR15">
-        <v>0.615199999999998</v>
+        <v>0.61519999999999797</v>
       </c>
       <c r="BS15">
         <v>1.095500000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:81">
+    <row r="16" spans="1:81" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B16">
-        <v>8.8508</v>
+        <v>8.8507999999999996</v>
       </c>
       <c r="C16">
         <v>10.9108</v>
       </c>
       <c r="D16">
-        <v>9.814299999999999</v>
+        <v>9.8142999999999994</v>
       </c>
       <c r="E16">
         <v>2.06</v>
@@ -2219,22 +2243,22 @@
         <v>0.9634999999999998</v>
       </c>
       <c r="G16">
-        <v>21.0983</v>
+        <v>21.098299999999998</v>
       </c>
       <c r="H16">
         <v>21.6523</v>
       </c>
       <c r="I16">
-        <v>19.5113</v>
+        <v>19.511299999999999</v>
       </c>
       <c r="J16">
-        <v>0.554000000000002</v>
+        <v>0.55400000000000205</v>
       </c>
       <c r="K16">
         <v>-1.587</v>
       </c>
       <c r="L16">
-        <v>9.658099999999999</v>
+        <v>9.6580999999999992</v>
       </c>
       <c r="M16">
         <v>10.98555</v>
@@ -2243,49 +2267,49 @@
         <v>9.9657</v>
       </c>
       <c r="O16">
-        <v>1.327450000000001</v>
+        <v>1.3274500000000009</v>
       </c>
       <c r="P16">
-        <v>0.3076000000000008</v>
+        <v>0.30760000000000082</v>
       </c>
       <c r="Q16">
-        <v>24.51565</v>
+        <v>24.515650000000001</v>
       </c>
       <c r="R16">
         <v>24.7209</v>
       </c>
       <c r="S16">
-        <v>24.89325</v>
+        <v>24.893249999999998</v>
       </c>
       <c r="T16">
-        <v>0.2052499999999995</v>
+        <v>0.20524999999999949</v>
       </c>
       <c r="U16">
-        <v>0.377600000000001</v>
+        <v>0.37760000000000099</v>
       </c>
       <c r="V16">
-        <v>7.5281</v>
+        <v>7.5281000000000002</v>
       </c>
       <c r="W16">
-        <v>9.012499999999999</v>
+        <v>9.0124999999999993</v>
       </c>
       <c r="X16">
-        <v>8.202400000000001</v>
+        <v>8.2024000000000008</v>
       </c>
       <c r="Y16">
-        <v>1.484399999999999</v>
+        <v>1.4843999999999991</v>
       </c>
       <c r="Z16">
-        <v>0.6743000000000006</v>
+        <v>0.67430000000000057</v>
       </c>
       <c r="AA16">
-        <v>22.562</v>
+        <v>22.562000000000001</v>
       </c>
       <c r="AB16">
         <v>22.4527</v>
       </c>
       <c r="AC16">
-        <v>20.7985</v>
+        <v>20.798500000000001</v>
       </c>
       <c r="AD16">
         <v>-0.1093000000000011</v>
@@ -2294,58 +2318,58 @@
         <v>-1.763500000000001</v>
       </c>
       <c r="AP16">
-        <v>9.873900000000001</v>
+        <v>9.8739000000000008</v>
       </c>
       <c r="AQ16">
         <v>11.8506</v>
       </c>
       <c r="AR16">
-        <v>10.6643</v>
+        <v>10.664300000000001</v>
       </c>
       <c r="AS16">
         <v>1.976699999999999</v>
       </c>
       <c r="AT16">
-        <v>0.7904</v>
+        <v>0.79039999999999999</v>
       </c>
       <c r="AU16">
-        <v>23.0963</v>
+        <v>23.096299999999999</v>
       </c>
       <c r="AV16">
         <v>23.276</v>
       </c>
       <c r="AW16">
-        <v>21.7299</v>
+        <v>21.729900000000001</v>
       </c>
       <c r="AX16">
-        <v>0.1797000000000004</v>
+        <v>0.17970000000000039</v>
       </c>
       <c r="AY16">
-        <v>-1.366399999999999</v>
+        <v>-1.3663999999999989</v>
       </c>
       <c r="BJ16">
-        <v>10.4852</v>
+        <v>10.485200000000001</v>
       </c>
       <c r="BK16">
-        <v>12.7129</v>
+        <v>12.712899999999999</v>
       </c>
       <c r="BL16">
         <v>11.2193</v>
       </c>
       <c r="BM16">
-        <v>2.227699999999999</v>
+        <v>2.2276999999999991</v>
       </c>
       <c r="BN16">
-        <v>0.7340999999999998</v>
+        <v>0.73409999999999975</v>
       </c>
       <c r="BO16">
-        <v>22.0041</v>
+        <v>22.004100000000001</v>
       </c>
       <c r="BP16">
-        <v>21.7071</v>
+        <v>21.707100000000001</v>
       </c>
       <c r="BQ16">
-        <v>19.8199</v>
+        <v>19.819900000000001</v>
       </c>
       <c r="BR16">
         <v>-0.2970000000000006</v>
@@ -2354,7 +2378,7 @@
         <v>-2.184200000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:81">
+    <row r="17" spans="1:81" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>31</v>
       </c>
@@ -2362,49 +2386,49 @@
         <v>7.61</v>
       </c>
       <c r="C17">
-        <v>8.4979</v>
+        <v>8.4978999999999996</v>
       </c>
       <c r="D17">
-        <v>7.4298</v>
+        <v>7.4298000000000002</v>
       </c>
       <c r="E17">
-        <v>0.8878999999999992</v>
+        <v>0.88789999999999925</v>
       </c>
       <c r="F17">
-        <v>-0.1802000000000001</v>
+        <v>-0.18020000000000011</v>
       </c>
       <c r="G17">
-        <v>23.1243</v>
+        <v>23.124300000000002</v>
       </c>
       <c r="H17">
-        <v>23.6198</v>
+        <v>23.619800000000001</v>
       </c>
       <c r="I17">
         <v>22.8705</v>
       </c>
       <c r="J17">
-        <v>0.4954999999999998</v>
+        <v>0.49549999999999977</v>
       </c>
       <c r="K17">
         <v>-0.2538000000000018</v>
       </c>
       <c r="L17">
-        <v>3.46695</v>
+        <v>3.4669500000000002</v>
       </c>
       <c r="M17">
-        <v>4.2935</v>
+        <v>4.2934999999999999</v>
       </c>
       <c r="N17">
-        <v>3.9973</v>
+        <v>3.9973000000000001</v>
       </c>
       <c r="O17">
-        <v>0.8265500000000001</v>
+        <v>0.82655000000000012</v>
       </c>
       <c r="P17">
-        <v>0.5303500000000003</v>
+        <v>0.53035000000000032</v>
       </c>
       <c r="Q17">
-        <v>20.09575</v>
+        <v>20.095749999999999</v>
       </c>
       <c r="R17">
         <v>19.93065</v>
@@ -2413,43 +2437,43 @@
         <v>20.0502</v>
       </c>
       <c r="T17">
-        <v>-0.1651000000000025</v>
+        <v>-0.16510000000000249</v>
       </c>
       <c r="U17">
-        <v>-0.0455500000000022</v>
+        <v>-4.55500000000022E-2</v>
       </c>
       <c r="AP17">
-        <v>10.2048</v>
+        <v>10.204800000000001</v>
       </c>
       <c r="AQ17">
-        <v>11.0993</v>
+        <v>11.099299999999999</v>
       </c>
       <c r="AR17">
-        <v>9.889699999999999</v>
+        <v>9.8896999999999995</v>
       </c>
       <c r="AS17">
-        <v>0.894499999999999</v>
+        <v>0.89449999999999896</v>
       </c>
       <c r="AT17">
-        <v>-0.315100000000001</v>
+        <v>-0.31510000000000099</v>
       </c>
       <c r="AU17">
         <v>23.73</v>
       </c>
       <c r="AV17">
-        <v>24.5176</v>
+        <v>24.517600000000002</v>
       </c>
       <c r="AW17">
-        <v>23.7674</v>
+        <v>23.767399999999999</v>
       </c>
       <c r="AX17">
-        <v>0.7876000000000012</v>
+        <v>0.78760000000000119</v>
       </c>
       <c r="AY17">
-        <v>0.0373999999999981</v>
+        <v>3.7399999999998101E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:81">
+    <row r="18" spans="1:81" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>32</v>
       </c>
@@ -2457,28 +2481,28 @@
         <v>10.8666</v>
       </c>
       <c r="C18">
-        <v>12.0645</v>
+        <v>12.064500000000001</v>
       </c>
       <c r="D18">
-        <v>11.5234</v>
+        <v>11.523400000000001</v>
       </c>
       <c r="E18">
-        <v>1.197900000000001</v>
+        <v>1.1979000000000011</v>
       </c>
       <c r="F18">
-        <v>0.6568000000000005</v>
+        <v>0.65680000000000049</v>
       </c>
       <c r="G18">
-        <v>25.4118</v>
+        <v>25.411799999999999</v>
       </c>
       <c r="H18">
-        <v>24.5363</v>
+        <v>24.536300000000001</v>
       </c>
       <c r="I18">
-        <v>25.0631</v>
+        <v>25.063099999999999</v>
       </c>
       <c r="J18">
-        <v>-0.8754999999999988</v>
+        <v>-0.87549999999999883</v>
       </c>
       <c r="K18">
         <v>-0.3487000000000009</v>
@@ -2490,188 +2514,188 @@
         <v>13.1798</v>
       </c>
       <c r="N18">
-        <v>11.9647</v>
+        <v>11.964700000000001</v>
       </c>
       <c r="O18">
         <v>1.5952</v>
       </c>
       <c r="P18">
-        <v>0.3801000000000005</v>
+        <v>0.38010000000000049</v>
       </c>
       <c r="Q18">
         <v>25.8705</v>
       </c>
       <c r="R18">
-        <v>25.9167</v>
+        <v>25.916699999999999</v>
       </c>
       <c r="S18">
         <v>25.4771</v>
       </c>
       <c r="T18">
-        <v>0.04619999999999891</v>
+        <v>4.6199999999998909E-2</v>
       </c>
       <c r="U18">
-        <v>-0.3933999999999997</v>
+        <v>-0.39339999999999969</v>
       </c>
     </row>
-    <row r="19" spans="1:81">
+    <row r="19" spans="1:81" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B19">
-        <v>7.9632</v>
+        <v>7.9631999999999996</v>
       </c>
       <c r="C19">
-        <v>7.9079</v>
+        <v>7.9078999999999997</v>
       </c>
       <c r="D19">
-        <v>6.8978</v>
+        <v>6.8978000000000002</v>
       </c>
       <c r="E19">
-        <v>-0.0552999999999999</v>
+        <v>-5.5299999999999898E-2</v>
       </c>
       <c r="F19">
         <v>-1.065399999999999</v>
       </c>
       <c r="G19">
-        <v>23.115</v>
+        <v>23.114999999999998</v>
       </c>
       <c r="H19">
-        <v>23.2479</v>
+        <v>23.247900000000001</v>
       </c>
       <c r="I19">
-        <v>23.4547</v>
+        <v>23.454699999999999</v>
       </c>
       <c r="J19">
         <v>0.1329000000000029</v>
       </c>
       <c r="K19">
-        <v>0.3397000000000006</v>
+        <v>0.33970000000000061</v>
       </c>
       <c r="L19">
-        <v>7.41055</v>
+        <v>7.4105499999999997</v>
       </c>
       <c r="M19">
-        <v>7.8517</v>
+        <v>7.8517000000000001</v>
       </c>
       <c r="N19">
         <v>7.0442</v>
       </c>
       <c r="O19">
-        <v>0.4411500000000004</v>
+        <v>0.44115000000000038</v>
       </c>
       <c r="P19">
-        <v>-0.3663499999999997</v>
+        <v>-0.36634999999999968</v>
       </c>
       <c r="Q19">
         <v>23.3277</v>
       </c>
       <c r="R19">
-        <v>23.70245</v>
+        <v>23.702449999999999</v>
       </c>
       <c r="S19">
-        <v>24.91715</v>
+        <v>24.917149999999999</v>
       </c>
       <c r="T19">
-        <v>0.3747499999999988</v>
+        <v>0.37474999999999881</v>
       </c>
       <c r="U19">
-        <v>1.589449999999999</v>
+        <v>1.5894499999999989</v>
       </c>
       <c r="AP19">
         <v>10.2598</v>
       </c>
       <c r="AQ19">
-        <v>10.2063</v>
+        <v>10.206300000000001</v>
       </c>
       <c r="AR19">
-        <v>9.119300000000001</v>
+        <v>9.1193000000000008</v>
       </c>
       <c r="AS19">
-        <v>-0.05349999999999966</v>
+        <v>-5.3499999999999659E-2</v>
       </c>
       <c r="AT19">
         <v>-1.140499999999999</v>
       </c>
       <c r="AU19">
-        <v>23.9212</v>
+        <v>23.921199999999999</v>
       </c>
       <c r="AV19">
-        <v>23.9673</v>
+        <v>23.967300000000002</v>
       </c>
       <c r="AW19">
         <v>24.0002</v>
       </c>
       <c r="AX19">
-        <v>0.04610000000000269</v>
+        <v>4.6100000000002687E-2</v>
       </c>
       <c r="AY19">
-        <v>0.07900000000000063</v>
+        <v>7.9000000000000625E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:81">
+    <row r="20" spans="1:81" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B20">
-        <v>8.298400000000001</v>
+        <v>8.2984000000000009</v>
       </c>
       <c r="C20">
-        <v>9.9184</v>
+        <v>9.9184000000000001</v>
       </c>
       <c r="D20">
-        <v>7.6214</v>
+        <v>7.6214000000000004</v>
       </c>
       <c r="E20">
         <v>1.619999999999999</v>
       </c>
       <c r="F20">
-        <v>-0.6770000000000005</v>
+        <v>-0.67700000000000049</v>
       </c>
       <c r="G20">
-        <v>22.3214</v>
+        <v>22.321400000000001</v>
       </c>
       <c r="H20">
-        <v>24.8745</v>
+        <v>24.874500000000001</v>
       </c>
       <c r="I20">
-        <v>24.1651</v>
+        <v>24.165099999999999</v>
       </c>
       <c r="J20">
         <v>2.553100000000001</v>
       </c>
       <c r="K20">
-        <v>1.843699999999998</v>
+        <v>1.8436999999999979</v>
       </c>
       <c r="L20">
-        <v>7.668900000000001</v>
+        <v>7.6689000000000007</v>
       </c>
       <c r="M20">
-        <v>8.803750000000001</v>
+        <v>8.8037500000000009</v>
       </c>
       <c r="N20">
-        <v>7.7194</v>
+        <v>7.7194000000000003</v>
       </c>
       <c r="O20">
-        <v>1.13485</v>
+        <v>1.1348499999999999</v>
       </c>
       <c r="P20">
-        <v>0.05049999999999955</v>
+        <v>5.0499999999999552E-2</v>
       </c>
       <c r="Q20">
-        <v>23.53065</v>
+        <v>23.530650000000001</v>
       </c>
       <c r="R20">
-        <v>23.82345</v>
+        <v>23.823450000000001</v>
       </c>
       <c r="S20">
         <v>24.60615</v>
       </c>
       <c r="T20">
-        <v>0.2927999999999997</v>
+        <v>0.29279999999999973</v>
       </c>
       <c r="U20">
-        <v>1.075499999999998</v>
+        <v>1.0754999999999979</v>
       </c>
       <c r="AP20">
         <v>11.2889</v>
@@ -2686,16 +2710,16 @@
         <v>1.638500000000001</v>
       </c>
       <c r="AT20">
-        <v>-0.8002000000000002</v>
+        <v>-0.80020000000000024</v>
       </c>
       <c r="AU20">
-        <v>23.3482</v>
+        <v>23.348199999999999</v>
       </c>
       <c r="AV20">
-        <v>26.5941</v>
+        <v>26.594100000000001</v>
       </c>
       <c r="AW20">
-        <v>24.9398</v>
+        <v>24.939800000000002</v>
       </c>
       <c r="AX20">
         <v>3.245900000000002</v>
@@ -2704,12 +2728,12 @@
         <v>1.591600000000003</v>
       </c>
     </row>
-    <row r="21" spans="1:81">
+    <row r="21" spans="1:81" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B21">
-        <v>10.7146</v>
+        <v>10.714600000000001</v>
       </c>
       <c r="C21">
         <v>10.8939</v>
@@ -2727,16 +2751,16 @@
         <v>25.529</v>
       </c>
       <c r="H21">
-        <v>25.1287</v>
+        <v>25.128699999999998</v>
       </c>
       <c r="I21">
         <v>25.5321</v>
       </c>
       <c r="J21">
-        <v>-0.4003000000000014</v>
+        <v>-0.40030000000000138</v>
       </c>
       <c r="K21">
-        <v>0.003099999999999881</v>
+        <v>3.0999999999998811E-3</v>
       </c>
       <c r="L21">
         <v>12.6577</v>
@@ -2748,72 +2772,72 @@
         <v>12.7591</v>
       </c>
       <c r="O21">
-        <v>0.4710000000000001</v>
+        <v>0.47100000000000009</v>
       </c>
       <c r="P21">
-        <v>0.1013999999999999</v>
+        <v>0.10139999999999991</v>
       </c>
       <c r="Q21">
-        <v>26.862</v>
+        <v>26.861999999999998</v>
       </c>
       <c r="R21">
-        <v>26.7305</v>
+        <v>26.730499999999999</v>
       </c>
       <c r="S21">
-        <v>26.9942</v>
+        <v>26.994199999999999</v>
       </c>
       <c r="T21">
-        <v>-0.1314999999999991</v>
+        <v>-0.13149999999999909</v>
       </c>
       <c r="U21">
-        <v>0.132200000000001</v>
+        <v>0.13220000000000101</v>
       </c>
     </row>
-    <row r="22" spans="1:81">
+    <row r="22" spans="1:81" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B22">
-        <v>0.36111</v>
+        <v>0.36110999999999999</v>
       </c>
       <c r="C22">
         <v>3.5951</v>
       </c>
       <c r="D22">
-        <v>0.24732</v>
+        <v>0.24732000000000001</v>
       </c>
       <c r="E22">
-        <v>3.23399</v>
+        <v>3.2339899999999999</v>
       </c>
       <c r="F22">
         <v>-0.11379</v>
       </c>
       <c r="G22">
-        <v>15.9493</v>
+        <v>15.949299999999999</v>
       </c>
       <c r="H22">
-        <v>13.761</v>
+        <v>13.760999999999999</v>
       </c>
       <c r="I22">
         <v>14.5817</v>
       </c>
       <c r="J22">
-        <v>-2.1883</v>
+        <v>-2.1882999999999999</v>
       </c>
       <c r="K22">
         <v>-1.367599999999999</v>
       </c>
       <c r="V22">
-        <v>4.9774</v>
+        <v>4.9774000000000003</v>
       </c>
       <c r="W22">
         <v>5.9615</v>
       </c>
       <c r="X22">
-        <v>4.7794</v>
+        <v>4.7793999999999999</v>
       </c>
       <c r="Y22">
-        <v>0.9840999999999998</v>
+        <v>0.98409999999999975</v>
       </c>
       <c r="Z22">
         <v>-0.1980000000000004</v>
@@ -2822,72 +2846,72 @@
         <v>20.0764</v>
       </c>
       <c r="AB22">
-        <v>21.1303</v>
+        <v>21.130299999999998</v>
       </c>
       <c r="AC22">
-        <v>20.2173</v>
+        <v>20.217300000000002</v>
       </c>
       <c r="AD22">
-        <v>1.053899999999999</v>
+        <v>1.0538999999999989</v>
       </c>
       <c r="AE22">
         <v>0.140900000000002</v>
       </c>
       <c r="BJ22">
-        <v>3.0009</v>
+        <v>3.0009000000000001</v>
       </c>
       <c r="BK22">
-        <v>5.9898</v>
+        <v>5.9897999999999998</v>
       </c>
       <c r="BL22">
         <v>2.8969</v>
       </c>
       <c r="BM22">
-        <v>2.9889</v>
+        <v>2.9889000000000001</v>
       </c>
       <c r="BN22">
-        <v>-0.1040000000000001</v>
+        <v>-0.10400000000000011</v>
       </c>
       <c r="BO22">
         <v>20.5246</v>
       </c>
       <c r="BP22">
-        <v>19.2519</v>
+        <v>19.251899999999999</v>
       </c>
       <c r="BQ22">
-        <v>19.6032</v>
+        <v>19.603200000000001</v>
       </c>
       <c r="BR22">
-        <v>-1.2727</v>
+        <v>-1.2726999999999999</v>
       </c>
       <c r="BS22">
-        <v>-0.9213999999999984</v>
+        <v>-0.92139999999999844</v>
       </c>
     </row>
-    <row r="23" spans="1:81">
+    <row r="23" spans="1:81" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B23">
-        <v>-0.64745</v>
+        <v>-0.64744999999999997</v>
       </c>
       <c r="C23">
-        <v>1.6739</v>
+        <v>1.6738999999999999</v>
       </c>
       <c r="D23">
-        <v>-0.12906</v>
+        <v>-0.12906000000000001</v>
       </c>
       <c r="E23">
-        <v>2.32135</v>
+        <v>2.3213499999999998</v>
       </c>
       <c r="F23">
-        <v>0.5183899999999999</v>
+        <v>0.51838999999999991</v>
       </c>
       <c r="G23">
         <v>10.5786</v>
       </c>
       <c r="H23">
-        <v>12.2292</v>
+        <v>12.229200000000001</v>
       </c>
       <c r="I23">
         <v>11.6076</v>
@@ -2896,19 +2920,19 @@
         <v>1.650600000000001</v>
       </c>
       <c r="K23">
-        <v>1.029</v>
+        <v>1.0289999999999999</v>
       </c>
       <c r="V23">
-        <v>4.4221</v>
+        <v>4.4221000000000004</v>
       </c>
       <c r="W23">
-        <v>4.7181</v>
+        <v>4.7180999999999997</v>
       </c>
       <c r="X23">
-        <v>5.7832</v>
+        <v>5.7831999999999999</v>
       </c>
       <c r="Y23">
-        <v>0.2959999999999994</v>
+        <v>0.29599999999999937</v>
       </c>
       <c r="Z23">
         <v>1.3611</v>
@@ -2917,105 +2941,105 @@
         <v>19.1114</v>
       </c>
       <c r="AB23">
-        <v>19.9641</v>
+        <v>19.964099999999998</v>
       </c>
       <c r="AC23">
-        <v>20.6214</v>
+        <v>20.621400000000001</v>
       </c>
       <c r="AD23">
-        <v>0.8526999999999987</v>
+        <v>0.85269999999999868</v>
       </c>
       <c r="AE23">
         <v>1.510000000000002</v>
       </c>
       <c r="BJ23">
-        <v>2.6303</v>
+        <v>2.6303000000000001</v>
       </c>
       <c r="BK23">
-        <v>4.1832</v>
+        <v>4.1832000000000003</v>
       </c>
       <c r="BL23">
-        <v>2.6977</v>
+        <v>2.6977000000000002</v>
       </c>
       <c r="BM23">
-        <v>1.5529</v>
+        <v>1.5528999999999999</v>
       </c>
       <c r="BN23">
-        <v>0.06740000000000013</v>
+        <v>6.7400000000000126E-2</v>
       </c>
       <c r="BO23">
         <v>15.2211</v>
       </c>
       <c r="BP23">
-        <v>16.3867</v>
+        <v>16.386700000000001</v>
       </c>
       <c r="BQ23">
-        <v>15.7145</v>
+        <v>15.714499999999999</v>
       </c>
       <c r="BR23">
-        <v>1.165600000000001</v>
+        <v>1.1656000000000011</v>
       </c>
       <c r="BS23">
-        <v>0.4933999999999994</v>
+        <v>0.49339999999999939</v>
       </c>
     </row>
-    <row r="24" spans="1:81">
+    <row r="24" spans="1:81" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B24">
-        <v>6.7258</v>
+        <v>6.7257999999999996</v>
       </c>
       <c r="C24">
-        <v>8.5885</v>
+        <v>8.5884999999999998</v>
       </c>
       <c r="D24">
-        <v>6.8672</v>
+        <v>6.8672000000000004</v>
       </c>
       <c r="E24">
         <v>1.8627</v>
       </c>
       <c r="F24">
-        <v>0.1414000000000009</v>
+        <v>0.14140000000000091</v>
       </c>
       <c r="G24">
         <v>22.7651</v>
       </c>
       <c r="H24">
-        <v>24.7008</v>
+        <v>24.700800000000001</v>
       </c>
       <c r="I24">
         <v>22.9772</v>
       </c>
       <c r="J24">
-        <v>1.935700000000001</v>
+        <v>1.9357000000000011</v>
       </c>
       <c r="K24">
-        <v>0.2120999999999995</v>
+        <v>0.21209999999999951</v>
       </c>
       <c r="BJ24">
-        <v>3.1857</v>
+        <v>3.1857000000000002</v>
       </c>
       <c r="BK24">
-        <v>5.2017</v>
+        <v>5.2016999999999998</v>
       </c>
       <c r="BL24">
-        <v>3.3015</v>
+        <v>3.3014999999999999</v>
       </c>
       <c r="BM24">
         <v>2.016</v>
       </c>
       <c r="BN24">
-        <v>0.1157999999999997</v>
+        <v>0.11579999999999969</v>
       </c>
       <c r="BO24">
-        <v>17.8025</v>
+        <v>17.802499999999998</v>
       </c>
       <c r="BP24">
-        <v>18.7917</v>
+        <v>18.791699999999999</v>
       </c>
       <c r="BQ24">
-        <v>17.9096</v>
+        <v>17.909600000000001</v>
       </c>
       <c r="BR24">
         <v>0.9892000000000003</v>
@@ -3024,84 +3048,84 @@
         <v>0.1071000000000026</v>
       </c>
     </row>
-    <row r="25" spans="1:81">
+    <row r="25" spans="1:81" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B25">
-        <v>5.5121</v>
+        <v>5.5121000000000002</v>
       </c>
       <c r="C25">
-        <v>7.0254</v>
+        <v>7.0254000000000003</v>
       </c>
       <c r="D25">
-        <v>6.0875</v>
+        <v>6.0875000000000004</v>
       </c>
       <c r="E25">
-        <v>1.5133</v>
+        <v>1.5133000000000001</v>
       </c>
       <c r="F25">
-        <v>0.5754000000000001</v>
+        <v>0.57540000000000013</v>
       </c>
       <c r="G25">
         <v>21.8658</v>
       </c>
       <c r="H25">
-        <v>24.0813</v>
+        <v>24.081299999999999</v>
       </c>
       <c r="I25">
-        <v>22.7037</v>
+        <v>22.703700000000001</v>
       </c>
       <c r="J25">
-        <v>2.215499999999999</v>
+        <v>2.2154999999999991</v>
       </c>
       <c r="K25">
         <v>0.8379000000000012</v>
       </c>
       <c r="V25">
-        <v>5.6503</v>
+        <v>5.6502999999999997</v>
       </c>
       <c r="W25">
-        <v>6.9515</v>
+        <v>6.9515000000000002</v>
       </c>
       <c r="X25">
-        <v>6.0726</v>
+        <v>6.0726000000000004</v>
       </c>
       <c r="Y25">
         <v>1.301200000000001</v>
       </c>
       <c r="Z25">
-        <v>0.4223000000000008</v>
+        <v>0.42230000000000079</v>
       </c>
       <c r="AA25">
-        <v>21.4485</v>
+        <v>21.448499999999999</v>
       </c>
       <c r="AB25">
         <v>23.4693</v>
       </c>
       <c r="AC25">
-        <v>22.2353</v>
+        <v>22.235299999999999</v>
       </c>
       <c r="AD25">
-        <v>2.020800000000001</v>
+        <v>2.0208000000000008</v>
       </c>
       <c r="AE25">
         <v>0.7867999999999995</v>
       </c>
       <c r="AF25">
-        <v>7.6705</v>
+        <v>7.6704999999999997</v>
       </c>
       <c r="AG25">
-        <v>8.872999999999999</v>
+        <v>8.8729999999999993</v>
       </c>
       <c r="AH25">
         <v>7.9497</v>
       </c>
       <c r="AI25">
-        <v>1.2025</v>
+        <v>1.2024999999999999</v>
       </c>
       <c r="AJ25">
-        <v>0.2792000000000003</v>
+        <v>0.27920000000000028</v>
       </c>
       <c r="AK25">
         <v>21.8553</v>
@@ -3110,171 +3134,171 @@
         <v>23.0793</v>
       </c>
       <c r="AM25">
-        <v>22.4168</v>
+        <v>22.416799999999999</v>
       </c>
       <c r="AN25">
         <v>1.224</v>
       </c>
       <c r="AO25">
-        <v>0.5614999999999988</v>
+        <v>0.56149999999999878</v>
       </c>
       <c r="AP25">
-        <v>9.772</v>
+        <v>9.7720000000000002</v>
       </c>
       <c r="AQ25">
-        <v>10.7985</v>
+        <v>10.798500000000001</v>
       </c>
       <c r="AR25">
-        <v>9.7913</v>
+        <v>9.7912999999999997</v>
       </c>
       <c r="AS25">
         <v>1.0265</v>
       </c>
       <c r="AT25">
-        <v>0.01929999999999943</v>
+        <v>1.9299999999999429E-2</v>
       </c>
       <c r="AU25">
-        <v>21.1667</v>
+        <v>21.166699999999999</v>
       </c>
       <c r="AV25">
         <v>22.0106</v>
       </c>
       <c r="AW25">
-        <v>21.2305</v>
+        <v>21.230499999999999</v>
       </c>
       <c r="AX25">
-        <v>0.8439000000000014</v>
+        <v>0.84390000000000143</v>
       </c>
       <c r="AY25">
-        <v>0.06380000000000052</v>
+        <v>6.3800000000000523E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:81">
+    <row r="26" spans="1:81" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B26">
-        <v>5.9122</v>
+        <v>5.9122000000000003</v>
       </c>
       <c r="C26">
-        <v>7.985</v>
+        <v>7.9850000000000003</v>
       </c>
       <c r="D26">
-        <v>5.8158</v>
+        <v>5.8158000000000003</v>
       </c>
       <c r="E26">
         <v>2.0728</v>
       </c>
       <c r="F26">
-        <v>-0.09640000000000004</v>
+        <v>-9.6400000000000041E-2</v>
       </c>
       <c r="G26">
-        <v>21.7658</v>
+        <v>21.765799999999999</v>
       </c>
       <c r="H26">
-        <v>24.1702</v>
+        <v>24.170200000000001</v>
       </c>
       <c r="I26">
-        <v>22.2037</v>
+        <v>22.203700000000001</v>
       </c>
       <c r="J26">
         <v>2.404400000000003</v>
       </c>
       <c r="K26">
-        <v>0.4379000000000026</v>
+        <v>0.43790000000000262</v>
       </c>
       <c r="V26">
-        <v>4.3721</v>
+        <v>4.3720999999999997</v>
       </c>
       <c r="W26">
-        <v>6.1565</v>
+        <v>6.1565000000000003</v>
       </c>
       <c r="X26">
-        <v>4.2451</v>
+        <v>4.2450999999999999</v>
       </c>
       <c r="Y26">
-        <v>1.784400000000001</v>
+        <v>1.7844000000000011</v>
       </c>
       <c r="Z26">
-        <v>-0.1269999999999998</v>
+        <v>-0.12699999999999981</v>
       </c>
       <c r="AA26">
-        <v>22.3745</v>
+        <v>22.374500000000001</v>
       </c>
       <c r="AB26">
-        <v>24.6763</v>
+        <v>24.676300000000001</v>
       </c>
       <c r="AC26">
-        <v>22.8378</v>
+        <v>22.837800000000001</v>
       </c>
       <c r="AD26">
-        <v>2.3018</v>
+        <v>2.3018000000000001</v>
       </c>
       <c r="AE26">
-        <v>0.4633000000000003</v>
+        <v>0.46330000000000032</v>
       </c>
       <c r="AP26">
-        <v>7.5434</v>
+        <v>7.5434000000000001</v>
       </c>
       <c r="AQ26">
-        <v>9.731999999999999</v>
+        <v>9.7319999999999993</v>
       </c>
       <c r="AR26">
-        <v>7.498</v>
+        <v>7.4980000000000002</v>
       </c>
       <c r="AS26">
-        <v>2.188599999999999</v>
+        <v>2.1885999999999992</v>
       </c>
       <c r="AT26">
-        <v>-0.04539999999999988</v>
+        <v>-4.5399999999999878E-2</v>
       </c>
       <c r="AU26">
-        <v>21.6918</v>
+        <v>21.691800000000001</v>
       </c>
       <c r="AV26">
         <v>23.581</v>
       </c>
       <c r="AW26">
-        <v>22.2247</v>
+        <v>22.224699999999999</v>
       </c>
       <c r="AX26">
-        <v>1.889199999999999</v>
+        <v>1.8891999999999991</v>
       </c>
       <c r="AY26">
-        <v>0.5328999999999979</v>
+        <v>0.53289999999999793</v>
       </c>
       <c r="BT26">
         <v>6.3525</v>
       </c>
       <c r="BU26">
-        <v>8.229200000000001</v>
+        <v>8.2292000000000005</v>
       </c>
       <c r="BV26">
-        <v>6.2154</v>
+        <v>6.2153999999999998</v>
       </c>
       <c r="BW26">
         <v>1.8767</v>
       </c>
       <c r="BX26">
-        <v>-0.1371000000000002</v>
+        <v>-0.13710000000000019</v>
       </c>
       <c r="BY26">
         <v>22.756</v>
       </c>
       <c r="BZ26">
-        <v>25.2309</v>
+        <v>25.230899999999998</v>
       </c>
       <c r="CA26">
-        <v>23.1395</v>
+        <v>23.139500000000002</v>
       </c>
       <c r="CB26">
-        <v>2.474899999999998</v>
+        <v>2.4748999999999981</v>
       </c>
       <c r="CC26">
-        <v>0.3835000000000015</v>
+        <v>0.38350000000000151</v>
       </c>
     </row>
-    <row r="27" spans="1:81">
+    <row r="27" spans="1:81" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>41</v>
       </c>
@@ -3285,132 +3309,132 @@
         <v>11.2898</v>
       </c>
       <c r="D27">
-        <v>10.1466</v>
+        <v>10.146599999999999</v>
       </c>
       <c r="E27">
-        <v>0.5260999999999996</v>
+        <v>0.52609999999999957</v>
       </c>
       <c r="F27">
-        <v>-0.6171000000000006</v>
+        <v>-0.61710000000000065</v>
       </c>
       <c r="G27">
-        <v>21.8708</v>
+        <v>21.870799999999999</v>
       </c>
       <c r="H27">
-        <v>21.7594</v>
+        <v>21.759399999999999</v>
       </c>
       <c r="I27">
-        <v>21.8084</v>
+        <v>21.808399999999999</v>
       </c>
       <c r="J27">
-        <v>-0.1113999999999997</v>
+        <v>-0.11139999999999969</v>
       </c>
       <c r="K27">
-        <v>-0.06240000000000023</v>
+        <v>-6.2400000000000233E-2</v>
       </c>
       <c r="AF27">
-        <v>9.139900000000001</v>
+        <v>9.1399000000000008</v>
       </c>
       <c r="AG27">
-        <v>9.682600000000001</v>
+        <v>9.6826000000000008</v>
       </c>
       <c r="AH27">
-        <v>8.4846</v>
+        <v>8.4846000000000004</v>
       </c>
       <c r="AI27">
-        <v>0.5427</v>
+        <v>0.54269999999999996</v>
       </c>
       <c r="AJ27">
-        <v>-0.6553000000000004</v>
+        <v>-0.65530000000000044</v>
       </c>
       <c r="AK27">
-        <v>22.3375</v>
+        <v>22.337499999999999</v>
       </c>
       <c r="AL27">
-        <v>22.1801</v>
+        <v>22.180099999999999</v>
       </c>
       <c r="AM27">
-        <v>22.341</v>
+        <v>22.341000000000001</v>
       </c>
       <c r="AN27">
         <v>-0.1573999999999991</v>
       </c>
       <c r="AO27">
-        <v>0.003500000000002501</v>
+        <v>3.5000000000025011E-3</v>
       </c>
       <c r="AP27">
-        <v>13.8105</v>
+        <v>13.810499999999999</v>
       </c>
       <c r="AQ27">
-        <v>14.3176</v>
+        <v>14.317600000000001</v>
       </c>
       <c r="AR27">
         <v>13.1829</v>
       </c>
       <c r="AS27">
-        <v>0.5071000000000012</v>
+        <v>0.50710000000000122</v>
       </c>
       <c r="AT27">
-        <v>-0.6275999999999993</v>
+        <v>-0.62759999999999927</v>
       </c>
       <c r="AU27">
-        <v>22.9324</v>
+        <v>22.932400000000001</v>
       </c>
       <c r="AV27">
-        <v>22.7079</v>
+        <v>22.707899999999999</v>
       </c>
       <c r="AW27">
         <v>22.81</v>
       </c>
       <c r="AX27">
-        <v>-0.2245000000000026</v>
+        <v>-0.22450000000000259</v>
       </c>
       <c r="AY27">
-        <v>-0.1224000000000025</v>
+        <v>-0.12240000000000251</v>
       </c>
       <c r="BT27">
-        <v>9.5078</v>
+        <v>9.5077999999999996</v>
       </c>
       <c r="BU27">
-        <v>9.906499999999999</v>
+        <v>9.9064999999999994</v>
       </c>
       <c r="BV27">
         <v>9.0183</v>
       </c>
       <c r="BW27">
-        <v>0.3986999999999998</v>
+        <v>0.39869999999999978</v>
       </c>
       <c r="BX27">
         <v>-0.4894999999999996</v>
       </c>
       <c r="BY27">
-        <v>23.4767</v>
+        <v>23.476700000000001</v>
       </c>
       <c r="BZ27">
-        <v>23.4275</v>
+        <v>23.427499999999998</v>
       </c>
       <c r="CA27">
-        <v>22.859</v>
+        <v>22.859000000000002</v>
       </c>
       <c r="CB27">
-        <v>-0.04920000000000258</v>
+        <v>-4.9200000000002582E-2</v>
       </c>
       <c r="CC27">
-        <v>-0.6176999999999992</v>
+        <v>-0.61769999999999925</v>
       </c>
     </row>
-    <row r="28" spans="1:81">
+    <row r="28" spans="1:81" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B28">
-        <v>5.8682</v>
+        <v>5.8681999999999999</v>
       </c>
       <c r="C28">
-        <v>7.4229</v>
+        <v>7.4229000000000003</v>
       </c>
       <c r="D28">
-        <v>7.3703</v>
+        <v>7.3703000000000003</v>
       </c>
       <c r="E28">
         <v>1.5547</v>
@@ -3419,159 +3443,159 @@
         <v>1.5021</v>
       </c>
       <c r="G28">
-        <v>22.2114</v>
+        <v>22.211400000000001</v>
       </c>
       <c r="H28">
-        <v>23.5568</v>
+        <v>23.556799999999999</v>
       </c>
       <c r="I28">
-        <v>24.2602</v>
+        <v>24.260200000000001</v>
       </c>
       <c r="J28">
-        <v>1.345399999999998</v>
+        <v>1.3453999999999979</v>
       </c>
       <c r="K28">
         <v>2.0488</v>
       </c>
       <c r="V28">
-        <v>7.1988</v>
+        <v>7.1988000000000003</v>
       </c>
       <c r="W28">
-        <v>7.5702</v>
+        <v>7.5701999999999998</v>
       </c>
       <c r="X28">
         <v>7.2919</v>
       </c>
       <c r="Y28">
-        <v>0.3713999999999995</v>
+        <v>0.37139999999999951</v>
       </c>
       <c r="Z28">
-        <v>0.09309999999999974</v>
+        <v>9.3099999999999739E-2</v>
       </c>
       <c r="AA28">
-        <v>21.7429</v>
+        <v>21.742899999999999</v>
       </c>
       <c r="AB28">
         <v>21.491</v>
       </c>
       <c r="AC28">
-        <v>21.3363</v>
+        <v>21.336300000000001</v>
       </c>
       <c r="AD28">
-        <v>-0.2518999999999991</v>
+        <v>-0.25189999999999912</v>
       </c>
       <c r="AE28">
-        <v>-0.4065999999999974</v>
+        <v>-0.40659999999999741</v>
       </c>
       <c r="AF28">
-        <v>4.0451</v>
+        <v>4.0450999999999997</v>
       </c>
       <c r="AG28">
-        <v>5.4294</v>
+        <v>5.4294000000000002</v>
       </c>
       <c r="AH28">
-        <v>5.8117</v>
+        <v>5.8117000000000001</v>
       </c>
       <c r="AI28">
         <v>1.384300000000001</v>
       </c>
       <c r="AJ28">
-        <v>1.7666</v>
+        <v>1.7665999999999999</v>
       </c>
       <c r="AK28">
-        <v>21.0629</v>
+        <v>21.062899999999999</v>
       </c>
       <c r="AL28">
         <v>22.8568</v>
       </c>
       <c r="AM28">
-        <v>23.0125</v>
+        <v>23.012499999999999</v>
       </c>
       <c r="AN28">
-        <v>1.793900000000001</v>
+        <v>1.7939000000000009</v>
       </c>
       <c r="AO28">
         <v>1.9496</v>
       </c>
       <c r="AZ28">
-        <v>6.5849</v>
+        <v>6.5849000000000002</v>
       </c>
       <c r="BA28">
-        <v>7.9751</v>
+        <v>7.9751000000000003</v>
       </c>
       <c r="BB28">
-        <v>7.9071</v>
+        <v>7.9070999999999998</v>
       </c>
       <c r="BC28">
-        <v>1.3902</v>
+        <v>1.3902000000000001</v>
       </c>
       <c r="BD28">
         <v>1.3222</v>
       </c>
       <c r="BE28">
-        <v>21.6732</v>
+        <v>21.673200000000001</v>
       </c>
       <c r="BF28">
-        <v>23.1796</v>
+        <v>23.179600000000001</v>
       </c>
       <c r="BG28">
         <v>23.0947</v>
       </c>
       <c r="BH28">
-        <v>1.506399999999999</v>
+        <v>1.5063999999999991</v>
       </c>
       <c r="BI28">
         <v>1.421499999999998</v>
       </c>
       <c r="BJ28">
-        <v>5.5266</v>
+        <v>5.5266000000000002</v>
       </c>
       <c r="BK28">
         <v>6.8243</v>
       </c>
       <c r="BL28">
-        <v>7.1238</v>
+        <v>7.1238000000000001</v>
       </c>
       <c r="BM28">
-        <v>1.2977</v>
+        <v>1.2977000000000001</v>
       </c>
       <c r="BN28">
         <v>1.5972</v>
       </c>
       <c r="BO28">
-        <v>22.5679</v>
+        <v>22.567900000000002</v>
       </c>
       <c r="BP28">
-        <v>24.0389</v>
+        <v>24.038900000000002</v>
       </c>
       <c r="BQ28">
-        <v>24.0222</v>
+        <v>24.022200000000002</v>
       </c>
       <c r="BR28">
-        <v>1.471</v>
+        <v>1.4710000000000001</v>
       </c>
       <c r="BS28">
-        <v>1.4543</v>
+        <v>1.4542999999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:81">
+    <row r="29" spans="1:81" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B29">
-        <v>5.6222</v>
+        <v>5.6222000000000003</v>
       </c>
       <c r="C29">
-        <v>7.154</v>
+        <v>7.1539999999999999</v>
       </c>
       <c r="D29">
-        <v>5.4362</v>
+        <v>5.4362000000000004</v>
       </c>
       <c r="E29">
-        <v>1.5318</v>
+        <v>1.5318000000000001</v>
       </c>
       <c r="F29">
-        <v>-0.1859999999999999</v>
+        <v>-0.18599999999999989</v>
       </c>
       <c r="G29">
         <v>22.8323</v>
@@ -3580,13 +3604,13 @@
         <v>23.2254</v>
       </c>
       <c r="I29">
-        <v>22.4578</v>
+        <v>22.457799999999999</v>
       </c>
       <c r="J29">
-        <v>0.3931000000000004</v>
+        <v>0.39310000000000039</v>
       </c>
       <c r="K29">
-        <v>-0.3745000000000012</v>
+        <v>-0.37450000000000122</v>
       </c>
       <c r="AF29">
         <v>3.9331</v>
@@ -3595,144 +3619,144 @@
         <v>5.2565</v>
       </c>
       <c r="AH29">
-        <v>3.7972</v>
+        <v>3.7972000000000001</v>
       </c>
       <c r="AI29">
-        <v>1.3234</v>
+        <v>1.3233999999999999</v>
       </c>
       <c r="AJ29">
-        <v>-0.1358999999999999</v>
+        <v>-0.13589999999999991</v>
       </c>
       <c r="AK29">
         <v>21.823</v>
       </c>
       <c r="AL29">
-        <v>22.7035</v>
+        <v>22.703499999999998</v>
       </c>
       <c r="AM29">
-        <v>21.3544</v>
+        <v>21.354399999999998</v>
       </c>
       <c r="AN29">
-        <v>0.8804999999999978</v>
+        <v>0.88049999999999784</v>
       </c>
       <c r="AO29">
-        <v>-0.4686000000000021</v>
+        <v>-0.46860000000000213</v>
       </c>
       <c r="AZ29">
-        <v>6.3052</v>
+        <v>6.3052000000000001</v>
       </c>
       <c r="BA29">
-        <v>7.8223</v>
+        <v>7.8223000000000003</v>
       </c>
       <c r="BB29">
-        <v>6.1736</v>
+        <v>6.1736000000000004</v>
       </c>
       <c r="BC29">
-        <v>1.5171</v>
+        <v>1.5170999999999999</v>
       </c>
       <c r="BD29">
-        <v>-0.1315999999999997</v>
+        <v>-0.13159999999999969</v>
       </c>
       <c r="BE29">
-        <v>22.6361</v>
+        <v>22.636099999999999</v>
       </c>
       <c r="BF29">
         <v>22.93</v>
       </c>
       <c r="BG29">
-        <v>22.292</v>
+        <v>22.292000000000002</v>
       </c>
       <c r="BH29">
-        <v>0.2939000000000007</v>
+        <v>0.29390000000000072</v>
       </c>
       <c r="BI29">
-        <v>-0.3440999999999974</v>
+        <v>-0.34409999999999741</v>
       </c>
       <c r="BJ29">
-        <v>5.4148</v>
+        <v>5.4147999999999996</v>
       </c>
       <c r="BK29">
-        <v>6.6582</v>
+        <v>6.6581999999999999</v>
       </c>
       <c r="BL29">
-        <v>5.2508</v>
+        <v>5.2507999999999999</v>
       </c>
       <c r="BM29">
-        <v>1.2434</v>
+        <v>1.2434000000000001</v>
       </c>
       <c r="BN29">
         <v>-0.1639999999999997</v>
       </c>
       <c r="BO29">
-        <v>23.2465</v>
+        <v>23.246500000000001</v>
       </c>
       <c r="BP29">
-        <v>23.9626</v>
+        <v>23.962599999999998</v>
       </c>
       <c r="BQ29">
         <v>22.8109</v>
       </c>
       <c r="BR29">
-        <v>0.7160999999999973</v>
+        <v>0.71609999999999729</v>
       </c>
       <c r="BS29">
-        <v>-0.4356000000000009</v>
+        <v>-0.43560000000000088</v>
       </c>
     </row>
-    <row r="30" spans="1:81">
+    <row r="30" spans="1:81" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B30">
-        <v>3.861</v>
+        <v>3.8610000000000002</v>
       </c>
       <c r="C30">
-        <v>6.9382</v>
+        <v>6.9382000000000001</v>
       </c>
       <c r="D30">
-        <v>5.2518</v>
+        <v>5.2518000000000002</v>
       </c>
       <c r="E30">
-        <v>3.0772</v>
+        <v>3.0771999999999999</v>
       </c>
       <c r="F30">
         <v>1.3908</v>
       </c>
       <c r="G30">
-        <v>17.5597</v>
+        <v>17.559699999999999</v>
       </c>
       <c r="H30">
-        <v>20.432</v>
+        <v>20.431999999999999</v>
       </c>
       <c r="I30">
-        <v>19.6101</v>
+        <v>19.610099999999999</v>
       </c>
       <c r="J30">
-        <v>2.872299999999999</v>
+        <v>2.8722999999999992</v>
       </c>
       <c r="K30">
-        <v>2.0504</v>
+        <v>2.0503999999999998</v>
       </c>
       <c r="V30">
-        <v>5.1615</v>
+        <v>5.1615000000000002</v>
       </c>
       <c r="W30">
         <v>6.5366</v>
       </c>
       <c r="X30">
-        <v>5.3659</v>
+        <v>5.3658999999999999</v>
       </c>
       <c r="Y30">
         <v>1.3751</v>
       </c>
       <c r="Z30">
-        <v>0.2043999999999997</v>
+        <v>0.20439999999999969</v>
       </c>
       <c r="AA30">
-        <v>18.9685</v>
+        <v>18.968499999999999</v>
       </c>
       <c r="AB30">
-        <v>20.5407</v>
+        <v>20.540700000000001</v>
       </c>
       <c r="AC30">
         <v>20.37865</v>
@@ -3747,46 +3771,46 @@
         <v>2.3306</v>
       </c>
       <c r="AG30">
-        <v>5.541</v>
+        <v>5.5410000000000004</v>
       </c>
       <c r="AH30">
         <v>3.9823</v>
       </c>
       <c r="AI30">
-        <v>3.2104</v>
+        <v>3.2103999999999999</v>
       </c>
       <c r="AJ30">
-        <v>1.6517</v>
+        <v>1.6516999999999999</v>
       </c>
       <c r="AK30">
         <v>15.1774</v>
       </c>
       <c r="AL30">
-        <v>18.8313</v>
+        <v>18.831299999999999</v>
       </c>
       <c r="AM30">
         <v>17.9877</v>
       </c>
       <c r="AN30">
-        <v>3.653899999999998</v>
+        <v>3.6538999999999979</v>
       </c>
       <c r="AO30">
-        <v>2.8103</v>
+        <v>2.8102999999999998</v>
       </c>
       <c r="AP30">
         <v>4.8731</v>
       </c>
       <c r="AQ30">
-        <v>8.4838</v>
+        <v>8.4838000000000005</v>
       </c>
       <c r="AR30">
-        <v>6.6221</v>
+        <v>6.6220999999999997</v>
       </c>
       <c r="AS30">
         <v>3.6107</v>
       </c>
       <c r="AT30">
-        <v>1.749</v>
+        <v>1.7490000000000001</v>
       </c>
       <c r="AU30">
         <v>17.6648</v>
@@ -3795,7 +3819,7 @@
         <v>20.1768</v>
       </c>
       <c r="AW30">
-        <v>19.4897</v>
+        <v>19.489699999999999</v>
       </c>
       <c r="AX30">
         <v>2.512</v>
@@ -3804,37 +3828,37 @@
         <v>1.8249</v>
       </c>
       <c r="BJ30">
-        <v>4.1812</v>
+        <v>4.1811999999999996</v>
       </c>
       <c r="BK30">
-        <v>7.7497</v>
+        <v>7.7496999999999998</v>
       </c>
       <c r="BL30">
-        <v>5.9206</v>
+        <v>5.9206000000000003</v>
       </c>
       <c r="BM30">
-        <v>3.5685</v>
+        <v>3.5684999999999998</v>
       </c>
       <c r="BN30">
-        <v>1.739400000000001</v>
+        <v>1.7394000000000009</v>
       </c>
       <c r="BO30">
         <v>17.2639</v>
       </c>
       <c r="BP30">
-        <v>20.0099</v>
+        <v>20.009899999999998</v>
       </c>
       <c r="BQ30">
         <v>19.1492</v>
       </c>
       <c r="BR30">
-        <v>2.745999999999999</v>
+        <v>2.7459999999999991</v>
       </c>
       <c r="BS30">
-        <v>1.885300000000001</v>
+        <v>1.8853000000000011</v>
       </c>
     </row>
-    <row r="31" spans="1:81">
+    <row r="31" spans="1:81" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>45</v>
       </c>
@@ -3848,28 +3872,28 @@
         <v>12.6981</v>
       </c>
       <c r="E31">
-        <v>0.3696999999999999</v>
+        <v>0.36969999999999992</v>
       </c>
       <c r="F31">
-        <v>-0.1798999999999999</v>
+        <v>-0.17989999999999989</v>
       </c>
       <c r="G31">
-        <v>25.3928</v>
+        <v>25.392800000000001</v>
       </c>
       <c r="H31">
-        <v>23.0467</v>
+        <v>23.046700000000001</v>
       </c>
       <c r="I31">
-        <v>23.8469</v>
+        <v>23.846900000000002</v>
       </c>
       <c r="J31">
-        <v>-2.3461</v>
+        <v>-2.3460999999999999</v>
       </c>
       <c r="K31">
-        <v>-1.5459</v>
+        <v>-1.5459000000000001</v>
       </c>
       <c r="L31">
-        <v>5.0565</v>
+        <v>5.0564999999999998</v>
       </c>
       <c r="M31">
         <v>5.4657</v>
@@ -3878,52 +3902,52 @@
         <v>4.8026</v>
       </c>
       <c r="O31">
-        <v>0.4092000000000002</v>
+        <v>0.40920000000000017</v>
       </c>
       <c r="P31">
-        <v>-0.2538999999999998</v>
+        <v>-0.25389999999999979</v>
       </c>
       <c r="Q31">
-        <v>20.0632</v>
+        <v>20.063199999999998</v>
       </c>
       <c r="R31">
-        <v>18.7113</v>
+        <v>18.711300000000001</v>
       </c>
       <c r="S31">
-        <v>18.8593</v>
+        <v>18.859300000000001</v>
       </c>
       <c r="T31">
         <v>-1.351899999999997</v>
       </c>
       <c r="U31">
-        <v>-1.203899999999997</v>
+        <v>-1.2038999999999971</v>
       </c>
       <c r="V31">
-        <v>6.4867</v>
+        <v>6.4866999999999999</v>
       </c>
       <c r="W31">
         <v>6.806</v>
       </c>
       <c r="X31">
-        <v>8.146800000000001</v>
+        <v>8.1468000000000007</v>
       </c>
       <c r="Y31">
-        <v>0.3193000000000001</v>
+        <v>0.31930000000000008</v>
       </c>
       <c r="Z31">
         <v>1.660100000000001</v>
       </c>
       <c r="AA31">
-        <v>21.2909</v>
+        <v>21.290900000000001</v>
       </c>
       <c r="AB31">
-        <v>21.5851</v>
+        <v>21.585100000000001</v>
       </c>
       <c r="AC31">
-        <v>22.8845</v>
+        <v>22.884499999999999</v>
       </c>
       <c r="AD31">
-        <v>0.2942</v>
+        <v>0.29420000000000002</v>
       </c>
       <c r="AE31">
         <v>1.593599999999999</v>
@@ -3932,43 +3956,43 @@
         <v>14.2818</v>
       </c>
       <c r="BA31">
-        <v>15.5766</v>
+        <v>15.576599999999999</v>
       </c>
       <c r="BB31">
-        <v>14.8168</v>
+        <v>14.816800000000001</v>
       </c>
       <c r="BC31">
-        <v>1.294799999999999</v>
+        <v>1.2947999999999991</v>
       </c>
       <c r="BD31">
-        <v>0.5350000000000001</v>
+        <v>0.53500000000000014</v>
       </c>
       <c r="BE31">
         <v>23.4589</v>
       </c>
       <c r="BF31">
-        <v>21.9502</v>
+        <v>21.950199999999999</v>
       </c>
       <c r="BG31">
-        <v>22.0662</v>
+        <v>22.066199999999998</v>
       </c>
       <c r="BH31">
         <v>-1.508700000000001</v>
       </c>
       <c r="BI31">
-        <v>-1.392700000000001</v>
+        <v>-1.3927000000000009</v>
       </c>
       <c r="BT31">
-        <v>9.955399999999999</v>
+        <v>9.9553999999999991</v>
       </c>
       <c r="BU31">
         <v>10.3507</v>
       </c>
       <c r="BV31">
-        <v>9.8454</v>
+        <v>9.8453999999999997</v>
       </c>
       <c r="BW31">
-        <v>0.3953000000000007</v>
+        <v>0.39530000000000071</v>
       </c>
       <c r="BX31">
         <v>-0.1099999999999994</v>
@@ -3980,16 +4004,16 @@
         <v>22.4785</v>
       </c>
       <c r="CA31">
-        <v>23.0155</v>
+        <v>23.015499999999999</v>
       </c>
       <c r="CB31">
-        <v>-1.8277</v>
+        <v>-1.8277000000000001</v>
       </c>
       <c r="CC31">
-        <v>-1.290700000000001</v>
+        <v>-1.2907000000000011</v>
       </c>
     </row>
-    <row r="32" spans="1:81">
+    <row r="32" spans="1:81" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>46</v>
       </c>
@@ -4000,13 +4024,13 @@
         <v>13.1591</v>
       </c>
       <c r="D32">
-        <v>12.4883</v>
+        <v>12.488300000000001</v>
       </c>
       <c r="E32">
-        <v>1.0235</v>
+        <v>1.0235000000000001</v>
       </c>
       <c r="F32">
-        <v>0.3527000000000005</v>
+        <v>0.35270000000000051</v>
       </c>
       <c r="G32">
         <v>25.4815</v>
@@ -4018,76 +4042,76 @@
         <v>24.1296</v>
       </c>
       <c r="J32">
-        <v>-0.8811</v>
+        <v>-0.88109999999999999</v>
       </c>
       <c r="K32">
         <v>-1.351900000000001</v>
       </c>
       <c r="L32">
-        <v>4.6858</v>
+        <v>4.6858000000000004</v>
       </c>
       <c r="M32">
-        <v>5.777</v>
+        <v>5.7770000000000001</v>
       </c>
       <c r="N32">
-        <v>5.0593</v>
+        <v>5.0593000000000004</v>
       </c>
       <c r="O32">
-        <v>1.0912</v>
+        <v>1.0911999999999999</v>
       </c>
       <c r="P32">
-        <v>0.3734999999999999</v>
+        <v>0.37349999999999989</v>
       </c>
       <c r="Q32">
-        <v>19.524</v>
+        <v>19.524000000000001</v>
       </c>
       <c r="R32">
-        <v>19.8632</v>
+        <v>19.863199999999999</v>
       </c>
       <c r="S32">
-        <v>18.4279</v>
+        <v>18.427900000000001</v>
       </c>
       <c r="T32">
-        <v>0.3391999999999982</v>
+        <v>0.33919999999999823</v>
       </c>
       <c r="U32">
-        <v>-1.0961</v>
+        <v>-1.0961000000000001</v>
       </c>
       <c r="V32">
-        <v>5.894</v>
+        <v>5.8940000000000001</v>
       </c>
       <c r="W32">
-        <v>6.293</v>
+        <v>6.2930000000000001</v>
       </c>
       <c r="X32">
         <v>5.4657</v>
       </c>
       <c r="Y32">
-        <v>0.399</v>
+        <v>0.39900000000000002</v>
       </c>
       <c r="Z32">
-        <v>-0.4283000000000001</v>
+        <v>-0.42830000000000013</v>
       </c>
       <c r="AA32">
-        <v>23.3303</v>
+        <v>23.330300000000001</v>
       </c>
       <c r="AB32">
-        <v>23.2511</v>
+        <v>23.251100000000001</v>
       </c>
       <c r="AC32">
-        <v>23.7907</v>
+        <v>23.790700000000001</v>
       </c>
       <c r="AD32">
-        <v>-0.07920000000000016</v>
+        <v>-7.9200000000000159E-2</v>
       </c>
       <c r="AE32">
-        <v>0.4603999999999999</v>
+        <v>0.46039999999999992</v>
       </c>
       <c r="AZ32">
-        <v>15.9538</v>
+        <v>15.953799999999999</v>
       </c>
       <c r="BA32">
-        <v>17.3847</v>
+        <v>17.384699999999999</v>
       </c>
       <c r="BB32">
         <v>16.7026</v>
@@ -4096,25 +4120,25 @@
         <v>1.430899999999999</v>
       </c>
       <c r="BD32">
-        <v>0.748800000000001</v>
+        <v>0.74880000000000102</v>
       </c>
       <c r="BE32">
         <v>24.8124</v>
       </c>
       <c r="BF32">
-        <v>24.237</v>
+        <v>24.236999999999998</v>
       </c>
       <c r="BG32">
-        <v>23.522</v>
+        <v>23.521999999999998</v>
       </c>
       <c r="BH32">
-        <v>-0.5754000000000019</v>
+        <v>-0.57540000000000191</v>
       </c>
       <c r="BI32">
         <v>-1.290400000000002</v>
       </c>
       <c r="BT32">
-        <v>11.1626</v>
+        <v>11.162599999999999</v>
       </c>
       <c r="BU32">
         <v>12.1158</v>
@@ -4123,42 +4147,42 @@
         <v>11.564</v>
       </c>
       <c r="BW32">
-        <v>0.9532000000000007</v>
+        <v>0.95320000000000071</v>
       </c>
       <c r="BX32">
-        <v>0.4014000000000006</v>
+        <v>0.40140000000000059</v>
       </c>
       <c r="BY32">
         <v>26.1248</v>
       </c>
       <c r="BZ32">
-        <v>25.7052</v>
+        <v>25.705200000000001</v>
       </c>
       <c r="CA32">
-        <v>25.4813</v>
+        <v>25.481300000000001</v>
       </c>
       <c r="CB32">
-        <v>-0.4195999999999991</v>
+        <v>-0.41959999999999908</v>
       </c>
       <c r="CC32">
-        <v>-0.6434999999999995</v>
+        <v>-0.64349999999999952</v>
       </c>
     </row>
-    <row r="33" spans="1:81">
+    <row r="33" spans="1:81" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B33">
-        <v>9.259</v>
+        <v>9.2590000000000003</v>
       </c>
       <c r="C33">
         <v>10.0314</v>
       </c>
       <c r="D33">
-        <v>9.121</v>
+        <v>9.1210000000000004</v>
       </c>
       <c r="E33">
-        <v>0.7723999999999993</v>
+        <v>0.77239999999999931</v>
       </c>
       <c r="F33">
         <v>-0.1379999999999999</v>
@@ -4170,91 +4194,91 @@
         <v>20.2376</v>
       </c>
       <c r="I33">
-        <v>19.7358</v>
+        <v>19.735800000000001</v>
       </c>
       <c r="J33">
         <v>0.5882000000000005</v>
       </c>
       <c r="K33">
-        <v>0.08640000000000114</v>
+        <v>8.6400000000001143E-2</v>
       </c>
       <c r="L33">
-        <v>5.8991</v>
+        <v>5.8990999999999998</v>
       </c>
       <c r="M33">
-        <v>6.5346</v>
+        <v>6.5346000000000002</v>
       </c>
       <c r="N33">
-        <v>5.8722</v>
+        <v>5.8722000000000003</v>
       </c>
       <c r="O33">
         <v>0.6355000000000004</v>
       </c>
       <c r="P33">
-        <v>-0.02689999999999948</v>
+        <v>-2.689999999999948E-2</v>
       </c>
       <c r="Q33">
-        <v>21.7248</v>
+        <v>21.724799999999998</v>
       </c>
       <c r="R33">
         <v>22.4405</v>
       </c>
       <c r="S33">
-        <v>22.246</v>
+        <v>22.245999999999999</v>
       </c>
       <c r="T33">
-        <v>0.7157000000000018</v>
+        <v>0.71570000000000178</v>
       </c>
       <c r="U33">
-        <v>0.5212000000000003</v>
+        <v>0.52120000000000033</v>
       </c>
       <c r="V33">
-        <v>6.6769</v>
+        <v>6.6768999999999998</v>
       </c>
       <c r="W33">
-        <v>6.1309</v>
+        <v>6.1308999999999996</v>
       </c>
       <c r="X33">
-        <v>5.9736</v>
+        <v>5.9736000000000002</v>
       </c>
       <c r="Y33">
-        <v>-0.5460000000000003</v>
+        <v>-0.54600000000000026</v>
       </c>
       <c r="Z33">
-        <v>-0.7032999999999996</v>
+        <v>-0.70329999999999959</v>
       </c>
       <c r="AA33">
-        <v>22.7534</v>
+        <v>22.753399999999999</v>
       </c>
       <c r="AB33">
-        <v>22.2798</v>
+        <v>22.279800000000002</v>
       </c>
       <c r="AC33">
-        <v>25.0049</v>
+        <v>25.004899999999999</v>
       </c>
       <c r="AD33">
-        <v>-0.4735999999999976</v>
+        <v>-0.47359999999999758</v>
       </c>
       <c r="AE33">
-        <v>2.2515</v>
+        <v>2.2515000000000001</v>
       </c>
       <c r="BT33">
-        <v>7.9387</v>
+        <v>7.9386999999999999</v>
       </c>
       <c r="BU33">
-        <v>8.8453</v>
+        <v>8.8452999999999999</v>
       </c>
       <c r="BV33">
-        <v>7.4868</v>
+        <v>7.4867999999999997</v>
       </c>
       <c r="BW33">
-        <v>0.9066000000000001</v>
+        <v>0.90660000000000007</v>
       </c>
       <c r="BX33">
-        <v>-0.4519000000000002</v>
+        <v>-0.45190000000000019</v>
       </c>
       <c r="BY33">
-        <v>20.4427</v>
+        <v>20.442699999999999</v>
       </c>
       <c r="BZ33">
         <v>21.6785</v>
@@ -4263,30 +4287,30 @@
         <v>20.2896</v>
       </c>
       <c r="CB33">
-        <v>1.235800000000001</v>
+        <v>1.2358000000000009</v>
       </c>
       <c r="CC33">
-        <v>-0.1530999999999985</v>
+        <v>-0.15309999999999849</v>
       </c>
     </row>
-    <row r="34" spans="1:81">
+    <row r="34" spans="1:81" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>48</v>
       </c>
       <c r="L34">
-        <v>5.5086</v>
+        <v>5.5086000000000004</v>
       </c>
       <c r="M34">
-        <v>5.8241</v>
+        <v>5.8240999999999996</v>
       </c>
       <c r="N34">
         <v>4.923</v>
       </c>
       <c r="O34">
-        <v>0.3154999999999992</v>
+        <v>0.31549999999999923</v>
       </c>
       <c r="P34">
-        <v>-0.5856000000000003</v>
+        <v>-0.58560000000000034</v>
       </c>
       <c r="Q34">
         <v>21.7073</v>
@@ -4295,10 +4319,10 @@
         <v>21.3398</v>
       </c>
       <c r="S34">
-        <v>20.4596</v>
+        <v>20.459599999999998</v>
       </c>
       <c r="T34">
-        <v>-0.3674999999999997</v>
+        <v>-0.36749999999999972</v>
       </c>
       <c r="U34">
         <v>-1.247700000000002</v>
@@ -4307,60 +4331,60 @@
         <v>6.7481</v>
       </c>
       <c r="BU34">
-        <v>7.2613</v>
+        <v>7.2613000000000003</v>
       </c>
       <c r="BV34">
-        <v>6.5656</v>
+        <v>6.5655999999999999</v>
       </c>
       <c r="BW34">
-        <v>0.5132000000000003</v>
+        <v>0.51320000000000032</v>
       </c>
       <c r="BX34">
-        <v>-0.1825000000000001</v>
+        <v>-0.18250000000000011</v>
       </c>
       <c r="BY34">
-        <v>23.0022</v>
+        <v>23.002199999999998</v>
       </c>
       <c r="BZ34">
-        <v>22.9028</v>
+        <v>22.902799999999999</v>
       </c>
       <c r="CA34">
-        <v>22.6059</v>
+        <v>22.605899999999998</v>
       </c>
       <c r="CB34">
-        <v>-0.09939999999999927</v>
+        <v>-9.9399999999999267E-2</v>
       </c>
       <c r="CC34">
         <v>-0.3963000000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:81">
+    <row r="35" spans="1:81" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B35">
-        <v>0.92369</v>
+        <v>0.92369000000000001</v>
       </c>
       <c r="C35">
-        <v>2.0392</v>
+        <v>2.0392000000000001</v>
       </c>
       <c r="D35">
-        <v>1.6809</v>
+        <v>1.6809000000000001</v>
       </c>
       <c r="E35">
         <v>1.11551</v>
       </c>
       <c r="F35">
-        <v>0.75721</v>
+        <v>0.75721000000000005</v>
       </c>
       <c r="G35">
-        <v>16.6588</v>
+        <v>16.658799999999999</v>
       </c>
       <c r="H35">
-        <v>18.2261</v>
+        <v>18.226099999999999</v>
       </c>
       <c r="I35">
-        <v>18.1609</v>
+        <v>18.160900000000002</v>
       </c>
       <c r="J35">
         <v>1.567299999999999</v>
@@ -4369,7 +4393,7 @@
         <v>1.502100000000002</v>
       </c>
     </row>
-    <row r="36" spans="1:81">
+    <row r="36" spans="1:81" ht="15" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>50</v>
       </c>
@@ -4386,85 +4410,85 @@
         <v>0.1164000000000005</v>
       </c>
       <c r="F36">
-        <v>0.05100000000000016</v>
+        <v>5.1000000000000163E-2</v>
       </c>
       <c r="G36">
-        <v>23.6107</v>
+        <v>23.610700000000001</v>
       </c>
       <c r="H36">
         <v>24.2957</v>
       </c>
       <c r="I36">
-        <v>23.7523</v>
+        <v>23.752300000000002</v>
       </c>
       <c r="J36">
-        <v>0.6849999999999987</v>
+        <v>0.68499999999999872</v>
       </c>
       <c r="K36">
-        <v>0.1416000000000004</v>
+        <v>0.14160000000000039</v>
       </c>
       <c r="L36">
-        <v>7.70605</v>
+        <v>7.7060500000000003</v>
       </c>
       <c r="M36">
-        <v>7.91625</v>
+        <v>7.9162499999999998</v>
       </c>
       <c r="N36">
-        <v>8.103949999999999</v>
+        <v>8.1039499999999993</v>
       </c>
       <c r="O36">
         <v>0.2101999999999995</v>
       </c>
       <c r="P36">
-        <v>0.397899999999999</v>
+        <v>0.39789999999999898</v>
       </c>
       <c r="Q36">
-        <v>19.8817</v>
+        <v>19.881699999999999</v>
       </c>
       <c r="R36">
-        <v>20.29085</v>
+        <v>20.290849999999999</v>
       </c>
       <c r="S36">
         <v>20.01145</v>
       </c>
       <c r="T36">
-        <v>0.4091499999999968</v>
+        <v>0.40914999999999679</v>
       </c>
       <c r="U36">
-        <v>0.1297500000000014</v>
+        <v>0.12975000000000139</v>
       </c>
       <c r="V36">
-        <v>6.736</v>
+        <v>6.7359999999999998</v>
       </c>
       <c r="W36">
-        <v>6.9856</v>
+        <v>6.9855999999999998</v>
       </c>
       <c r="X36">
         <v>7.1856</v>
       </c>
       <c r="Y36">
-        <v>0.2496</v>
+        <v>0.24959999999999999</v>
       </c>
       <c r="Z36">
-        <v>0.4496000000000002</v>
+        <v>0.44960000000000022</v>
       </c>
       <c r="AA36">
         <v>19.9556</v>
       </c>
       <c r="AB36">
-        <v>20.1467</v>
+        <v>20.146699999999999</v>
       </c>
       <c r="AC36">
-        <v>20.0126</v>
+        <v>20.012599999999999</v>
       </c>
       <c r="AD36">
-        <v>0.1910999999999987</v>
+        <v>0.19109999999999869</v>
       </c>
       <c r="AE36">
-        <v>0.05699999999999861</v>
+        <v>5.6999999999998607E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:81">
+    <row r="37" spans="1:81" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>51</v>
       </c>
@@ -4472,52 +4496,52 @@
         <v>11.5046</v>
       </c>
       <c r="C37">
-        <v>11.6041</v>
+        <v>11.604100000000001</v>
       </c>
       <c r="D37">
-        <v>9.0909</v>
+        <v>9.0908999999999995</v>
       </c>
       <c r="E37">
-        <v>0.09950000000000081</v>
+        <v>9.950000000000081E-2</v>
       </c>
       <c r="F37">
         <v>-2.4137</v>
       </c>
       <c r="G37">
-        <v>21.2085</v>
+        <v>21.208500000000001</v>
       </c>
       <c r="H37">
-        <v>22.6563</v>
+        <v>22.656300000000002</v>
       </c>
       <c r="I37">
-        <v>22.7381</v>
+        <v>22.738099999999999</v>
       </c>
       <c r="J37">
-        <v>1.447800000000001</v>
+        <v>1.4478000000000011</v>
       </c>
       <c r="K37">
         <v>1.529599999999999</v>
       </c>
       <c r="L37">
-        <v>6.800750000000001</v>
+        <v>6.8007500000000007</v>
       </c>
       <c r="M37">
-        <v>6.880599999999999</v>
+        <v>6.8805999999999994</v>
       </c>
       <c r="N37">
-        <v>5.91855</v>
+        <v>5.9185499999999998</v>
       </c>
       <c r="O37">
-        <v>0.07984999999999864</v>
+        <v>7.9849999999998644E-2</v>
       </c>
       <c r="P37">
-        <v>-0.882200000000001</v>
+        <v>-0.88220000000000098</v>
       </c>
       <c r="Q37">
-        <v>19.2752</v>
+        <v>19.275200000000002</v>
       </c>
       <c r="R37">
-        <v>20.08505</v>
+        <v>20.085049999999999</v>
       </c>
       <c r="S37">
         <v>20.41675</v>
@@ -4526,31 +4550,31 @@
         <v>0.8098500000000044</v>
       </c>
       <c r="U37">
-        <v>1.141550000000002</v>
+        <v>1.1415500000000021</v>
       </c>
       <c r="BT37">
-        <v>8.3072</v>
+        <v>8.3071999999999999</v>
       </c>
       <c r="BU37">
-        <v>9.3818</v>
+        <v>9.3818000000000001</v>
       </c>
       <c r="BV37">
-        <v>6.9636</v>
+        <v>6.9635999999999996</v>
       </c>
       <c r="BW37">
         <v>1.0746</v>
       </c>
       <c r="BX37">
-        <v>-1.3436</v>
+        <v>-1.3435999999999999</v>
       </c>
       <c r="BY37">
-        <v>19.3041</v>
+        <v>19.304099999999998</v>
       </c>
       <c r="BZ37">
         <v>20.2197</v>
       </c>
       <c r="CA37">
-        <v>21.1271</v>
+        <v>21.127099999999999</v>
       </c>
       <c r="CB37">
         <v>0.9156000000000013</v>
@@ -4559,7 +4583,7 @@
         <v>1.823</v>
       </c>
     </row>
-    <row r="38" spans="1:81">
+    <row r="38" spans="1:81" ht="15" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>52</v>
       </c>
@@ -4573,49 +4597,49 @@
         <v>11.945</v>
       </c>
       <c r="E38">
-        <v>0.08469999999999978</v>
+        <v>8.4699999999999775E-2</v>
       </c>
       <c r="F38">
         <v>-0.3254999999999999</v>
       </c>
       <c r="G38">
-        <v>23.3417</v>
+        <v>23.341699999999999</v>
       </c>
       <c r="H38">
-        <v>24.5888</v>
+        <v>24.588799999999999</v>
       </c>
       <c r="I38">
-        <v>24.0858</v>
+        <v>24.085799999999999</v>
       </c>
       <c r="J38">
-        <v>1.2471</v>
+        <v>1.2471000000000001</v>
       </c>
       <c r="K38">
-        <v>0.7440999999999995</v>
+        <v>0.74409999999999954</v>
       </c>
       <c r="L38">
-        <v>8.5098</v>
+        <v>8.5098000000000003</v>
       </c>
       <c r="M38">
-        <v>8.5603</v>
+        <v>8.5602999999999998</v>
       </c>
       <c r="N38">
         <v>8.1509</v>
       </c>
       <c r="O38">
-        <v>0.05049999999999955</v>
+        <v>5.0499999999999552E-2</v>
       </c>
       <c r="P38">
-        <v>-0.3589000000000002</v>
+        <v>-0.35890000000000022</v>
       </c>
       <c r="Q38">
-        <v>20.1167</v>
+        <v>20.116700000000002</v>
       </c>
       <c r="R38">
-        <v>21.1376</v>
+        <v>21.137599999999999</v>
       </c>
       <c r="S38">
-        <v>20.7274</v>
+        <v>20.727399999999999</v>
       </c>
       <c r="T38">
         <v>1.020899999999997</v>
@@ -4626,11 +4650,9 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B1:K1"/>
-    <mergeCell ref="L1:U1"/>
-    <mergeCell ref="V1:AE1"/>
-    <mergeCell ref="AF1:AO1"/>
-    <mergeCell ref="AP1:AY1"/>
+    <mergeCell ref="BO2:BS2"/>
+    <mergeCell ref="BT2:BX2"/>
+    <mergeCell ref="BY2:CC2"/>
     <mergeCell ref="AZ1:BI1"/>
     <mergeCell ref="BJ1:BS1"/>
     <mergeCell ref="BT1:CC1"/>
@@ -4647,9 +4669,11 @@
     <mergeCell ref="AZ2:BD2"/>
     <mergeCell ref="BE2:BI2"/>
     <mergeCell ref="BJ2:BN2"/>
-    <mergeCell ref="BO2:BS2"/>
-    <mergeCell ref="BT2:BX2"/>
-    <mergeCell ref="BY2:CC2"/>
+    <mergeCell ref="B1:K1"/>
+    <mergeCell ref="L1:U1"/>
+    <mergeCell ref="V1:AE1"/>
+    <mergeCell ref="AF1:AO1"/>
+    <mergeCell ref="AP1:AY1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>